<commit_message>
prepare for 2 cateogry experiment
</commit_message>
<xml_diff>
--- a/convParameters.xlsx
+++ b/convParameters.xlsx
@@ -247,7 +247,7 @@
     <t xml:space="preserve">EH</t>
   </si>
   <si>
-    <t xml:space="preserve">{4000,4000)</t>
+    <t xml:space="preserve">‘{4000,4000}’</t>
   </si>
   <si>
     <t xml:space="preserve">dontPad</t>
@@ -14392,8 +14392,8 @@
   </sheetPr>
   <dimension ref="A1:BK103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF2" activeCellId="0" sqref="AF2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W3" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD3" activeCellId="0" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14684,7 +14684,7 @@
       </c>
       <c r="AH3" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B3,AI3,AJ3,AK3,AL3,AM3,AN3,AO3,AP3,AQ3,AR3,AS3,AT3,AU3,AV3,AW3,AX3,AY3,AZ3,BA3,BB3,BC3,BD3,BE3,BF3,BG3,BH3,BI3,BJ3,BK3,BL3)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH0 --learningRate 0.1 --maxEpoch 100 --activation Tanh --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH0 --learningRate 0.1 --maxEpoch 100 --activation Tanh --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI3" s="0" t="str">
         <f aca="false">IF(D3="y", " --"&amp;D$1,IF(NOT(ISBLANK(D3))," --"&amp;D$1&amp;" "&amp;D3,""))</f>
@@ -14792,7 +14792,7 @@
       </c>
       <c r="BI3" s="0" t="str">
         <f aca="false">IF(AD3="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD3))," --"&amp;AD$1&amp;" "&amp;AD3,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ3" s="0" t="str">
         <f aca="false">IF(AE3="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE3))," --"&amp;AE$1&amp;" "&amp;AE3,""))</f>
@@ -14818,7 +14818,7 @@
       </c>
       <c r="AH4" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B4,AI4,AJ4,AK4,AL4,AM4,AN4,AO4,AP4,AQ4,AR4,AS4,AT4,AU4,AV4,AW4,AX4,AY4,AZ4,BA4,BB4,BC4,BD4,BE4,BF4,BG4,BH4,BI4,BJ4,BK4,BL4)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH1 --maxEpoch 100 --activation Tanh --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH1 --maxEpoch 100 --activation Tanh --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI4" s="0" t="str">
         <f aca="false">IF(D4="y", " --"&amp;D$1,IF(NOT(ISBLANK(D4))," --"&amp;D$1&amp;" "&amp;D4,""))</f>
@@ -14926,7 +14926,7 @@
       </c>
       <c r="BI4" s="0" t="str">
         <f aca="false">IF(AD4="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD4))," --"&amp;AD$1&amp;" "&amp;AD4,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ4" s="0" t="str">
         <f aca="false">IF(AE4="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE4))," --"&amp;AE$1&amp;" "&amp;AE4,""))</f>
@@ -14952,7 +14952,7 @@
       </c>
       <c r="AH5" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B5,AI5,AJ5,AK5,AL5,AM5,AN5,AO5,AP5,AQ5,AR5,AS5,AT5,AU5,AV5,AW5,AX5,AY5,AZ5,BA5,BB5,BC5,BD5,BE5,BF5,BG5,BH5,BI5,BJ5,BK5,BL5)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH2 --maxEpoch 10000 --activation Tanh --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH2 --maxEpoch 10000 --activation Tanh --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI5" s="0" t="str">
         <f aca="false">IF(D5="y", " --"&amp;D$1,IF(NOT(ISBLANK(D5))," --"&amp;D$1&amp;" "&amp;D5,""))</f>
@@ -15060,7 +15060,7 @@
       </c>
       <c r="BI5" s="0" t="str">
         <f aca="false">IF(AD5="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD5))," --"&amp;AD$1&amp;" "&amp;AD5,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ5" s="0" t="str">
         <f aca="false">IF(AE5="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE5))," --"&amp;AE$1&amp;" "&amp;AE5,""))</f>
@@ -15071,7 +15071,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>3</v>
       </c>
@@ -15089,7 +15089,7 @@
       </c>
       <c r="AH6" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B6,AI6,AJ6,AK6,AL6,AM6,AN6,AO6,AP6,AQ6,AR6,AS6,AT6,AU6,AV6,AW6,AX6,AY6,AZ6,BA6,BB6,BC6,BD6,BE6,BF6,BG6,BH6,BI6,BJ6,BK6,BL6)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH3 --maxEpoch 10000 --activation Tanh --hiddenSize {4000,4000) --dropout</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH3 --maxEpoch 10000 --activation Tanh --hiddenSize ‘{4000,4000}’ --dropout</v>
       </c>
       <c r="AI6" s="0" t="str">
         <f aca="false">IF(D6="y", " --"&amp;D$1,IF(NOT(ISBLANK(D6))," --"&amp;D$1&amp;" "&amp;D6,""))</f>
@@ -15197,7 +15197,7 @@
       </c>
       <c r="BI6" s="0" t="str">
         <f aca="false">IF(AD6="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD6))," --"&amp;AD$1&amp;" "&amp;AD6,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ6" s="0" t="str">
         <f aca="false">IF(AE6="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE6))," --"&amp;AE$1&amp;" "&amp;AE6,""))</f>
@@ -15223,7 +15223,7 @@
       </c>
       <c r="AH7" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B7,AI7,AJ7,AK7,AL7,AM7,AN7,AO7,AP7,AQ7,AR7,AS7,AT7,AU7,AV7,AW7,AX7,AY7,AZ7,BA7,BB7,BC7,BD7,BE7,BF7,BG7,BH7,BI7,BJ7,BK7,BL7)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH4 --maxEpoch 10000 --activation ReLU --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH4 --maxEpoch 10000 --activation ReLU --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI7" s="0" t="str">
         <f aca="false">IF(D7="y", " --"&amp;D$1,IF(NOT(ISBLANK(D7))," --"&amp;D$1&amp;" "&amp;D7,""))</f>
@@ -15331,7 +15331,7 @@
       </c>
       <c r="BI7" s="0" t="str">
         <f aca="false">IF(AD7="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD7))," --"&amp;AD$1&amp;" "&amp;AD7,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ7" s="0" t="str">
         <f aca="false">IF(AE7="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE7))," --"&amp;AE$1&amp;" "&amp;AE7,""))</f>
@@ -15342,7 +15342,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
         <v>5</v>
       </c>
@@ -15360,7 +15360,7 @@
       </c>
       <c r="AH8" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B8,AI8,AJ8,AK8,AL8,AM8,AN8,AO8,AP8,AQ8,AR8,AS8,AT8,AU8,AV8,AW8,AX8,AY8,AZ8,BA8,BB8,BC8,BD8,BE8,BF8,BG8,BH8,BI8,BJ8,BK8,BL8)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH5 --maxEpoch 10000 --activation ReLU --hiddenSize {4000,4000) --dropout</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH5 --maxEpoch 10000 --activation ReLU --hiddenSize ‘{4000,4000}’ --dropout</v>
       </c>
       <c r="AI8" s="0" t="str">
         <f aca="false">IF(D8="y", " --"&amp;D$1,IF(NOT(ISBLANK(D8))," --"&amp;D$1&amp;" "&amp;D8,""))</f>
@@ -15468,7 +15468,7 @@
       </c>
       <c r="BI8" s="0" t="str">
         <f aca="false">IF(AD8="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD8))," --"&amp;AD$1&amp;" "&amp;AD8,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ8" s="0" t="str">
         <f aca="false">IF(AE8="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE8))," --"&amp;AE$1&amp;" "&amp;AE8,""))</f>
@@ -15497,7 +15497,7 @@
       </c>
       <c r="AH9" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B9,AI9,AJ9,AK9,AL9,AM9,AN9,AO9,AP9,AQ9,AR9,AS9,AT9,AU9,AV9,AW9,AX9,AY9,AZ9,BA9,BB9,BC9,BD9,BE9,BF9,BG9,BH9,BI9,BJ9,BK9,BL9)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH6 --maxEpoch 10000 --activation Sigmoid --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH6 --maxEpoch 10000 --activation Sigmoid --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI9" s="0" t="str">
         <f aca="false">IF(D9="y", " --"&amp;D$1,IF(NOT(ISBLANK(D9))," --"&amp;D$1&amp;" "&amp;D9,""))</f>
@@ -15605,7 +15605,7 @@
       </c>
       <c r="BI9" s="0" t="str">
         <f aca="false">IF(AD9="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD9))," --"&amp;AD$1&amp;" "&amp;AD9,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ9" s="0" t="str">
         <f aca="false">IF(AE9="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE9))," --"&amp;AE$1&amp;" "&amp;AE9,""))</f>
@@ -15616,7 +15616,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
         <v>7</v>
       </c>
@@ -15637,7 +15637,7 @@
       </c>
       <c r="AH10" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B10,AI10,AJ10,AK10,AL10,AM10,AN10,AO10,AP10,AQ10,AR10,AS10,AT10,AU10,AV10,AW10,AX10,AY10,AZ10,BA10,BB10,BC10,BD10,BE10,BF10,BG10,BH10,BI10,BJ10,BK10,BL10)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH7 --maxEpoch 10000 --activation Sigmoid --hiddenSize {4000,4000) --dropout</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH7 --maxEpoch 10000 --activation Sigmoid --hiddenSize ‘{4000,4000}’ --dropout</v>
       </c>
       <c r="AI10" s="0" t="str">
         <f aca="false">IF(D10="y", " --"&amp;D$1,IF(NOT(ISBLANK(D10))," --"&amp;D$1&amp;" "&amp;D10,""))</f>
@@ -15745,7 +15745,7 @@
       </c>
       <c r="BI10" s="0" t="str">
         <f aca="false">IF(AD10="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD10))," --"&amp;AD$1&amp;" "&amp;AD10,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ10" s="0" t="str">
         <f aca="false">IF(AE10="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE10))," --"&amp;AE$1&amp;" "&amp;AE10,""))</f>
@@ -15756,7 +15756,7 @@
         <v> --dropout</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
         <v>8</v>
       </c>
@@ -15765,7 +15765,7 @@
       </c>
       <c r="AH11" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B11,AI11,AJ11,AK11,AL11,AM11,AN11,AO11,AP11,AQ11,AR11,AS11,AT11,AU11,AV11,AW11,AX11,AY11,AZ11,BA11,BB11,BC11,BD11,BE11,BF11,BG11,BH11,BI11,BJ11,BK11,BL11)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH8 --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH8 --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI11" s="0" t="str">
         <f aca="false">IF(D11="y", " --"&amp;D$1,IF(NOT(ISBLANK(D11))," --"&amp;D$1&amp;" "&amp;D11,""))</f>
@@ -15873,7 +15873,7 @@
       </c>
       <c r="BI11" s="0" t="str">
         <f aca="false">IF(AD11="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD11))," --"&amp;AD$1&amp;" "&amp;AD11,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ11" s="0" t="str">
         <f aca="false">IF(AE11="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE11))," --"&amp;AE$1&amp;" "&amp;AE11,""))</f>
@@ -15884,7 +15884,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
         <v>9</v>
       </c>
@@ -15896,7 +15896,7 @@
       </c>
       <c r="AH12" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B12,AI12,AJ12,AK12,AL12,AM12,AN12,AO12,AP12,AQ12,AR12,AS12,AT12,AU12,AV12,AW12,AX12,AY12,AZ12,BA12,BB12,BC12,BD12,BE12,BF12,BG12,BH12,BI12,BJ12,BK12,BL12)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH9 --zca --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH9 --zca --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI12" s="0" t="str">
         <f aca="false">IF(D12="y", " --"&amp;D$1,IF(NOT(ISBLANK(D12))," --"&amp;D$1&amp;" "&amp;D12,""))</f>
@@ -16004,7 +16004,7 @@
       </c>
       <c r="BI12" s="0" t="str">
         <f aca="false">IF(AD12="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD12))," --"&amp;AD$1&amp;" "&amp;AD12,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ12" s="0" t="str">
         <f aca="false">IF(AE12="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE12))," --"&amp;AE$1&amp;" "&amp;AE12,""))</f>
@@ -16015,7 +16015,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
         <v>10</v>
       </c>
@@ -16027,7 +16027,7 @@
       </c>
       <c r="AH13" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B13,AI13,AJ13,AK13,AL13,AM13,AN13,AO13,AP13,AQ13,AR13,AS13,AT13,AU13,AV13,AW13,AX13,AY13,AZ13,BA13,BB13,BC13,BD13,BE13,BF13,BG13,BH13,BI13,BJ13,BK13,BL13)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH10 --lecunlcn --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH10 --lecunlcn --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI13" s="0" t="str">
         <f aca="false">IF(D13="y", " --"&amp;D$1,IF(NOT(ISBLANK(D13))," --"&amp;D$1&amp;" "&amp;D13,""))</f>
@@ -16135,7 +16135,7 @@
       </c>
       <c r="BI13" s="0" t="str">
         <f aca="false">IF(AD13="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD13))," --"&amp;AD$1&amp;" "&amp;AD13,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ13" s="0" t="str">
         <f aca="false">IF(AE13="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE13))," --"&amp;AE$1&amp;" "&amp;AE13,""))</f>
@@ -16146,7 +16146,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
         <v>11</v>
       </c>
@@ -16161,7 +16161,7 @@
       </c>
       <c r="AH14" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B14,AI14,AJ14,AK14,AL14,AM14,AN14,AO14,AP14,AQ14,AR14,AS14,AT14,AU14,AV14,AW14,AX14,AY14,AZ14,BA14,BB14,BC14,BD14,BE14,BF14,BG14,BH14,BI14,BJ14,BK14,BL14)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH11 --zca --lecunlcn --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH11 --zca --lecunlcn --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI14" s="0" t="str">
         <f aca="false">IF(D14="y", " --"&amp;D$1,IF(NOT(ISBLANK(D14))," --"&amp;D$1&amp;" "&amp;D14,""))</f>
@@ -16269,7 +16269,7 @@
       </c>
       <c r="BI14" s="0" t="str">
         <f aca="false">IF(AD14="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD14))," --"&amp;AD$1&amp;" "&amp;AD14,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ14" s="0" t="str">
         <f aca="false">IF(AE14="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE14))," --"&amp;AE$1&amp;" "&amp;AE14,""))</f>
@@ -16280,7 +16280,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
         <v>12</v>
       </c>
@@ -16292,7 +16292,7 @@
       </c>
       <c r="AH15" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B15,AI15,AJ15,AK15,AL15,AM15,AN15,AO15,AP15,AQ15,AR15,AS15,AT15,AU15,AV15,AW15,AX15,AY15,AZ15,BA15,BB15,BC15,BD15,BE15,BF15,BG15,BH15,BI15,BJ15,BK15,BL15)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH12 --standardize --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH12 --standardize --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI15" s="0" t="str">
         <f aca="false">IF(D15="y", " --"&amp;D$1,IF(NOT(ISBLANK(D15))," --"&amp;D$1&amp;" "&amp;D15,""))</f>
@@ -16400,7 +16400,7 @@
       </c>
       <c r="BI15" s="0" t="str">
         <f aca="false">IF(AD15="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD15))," --"&amp;AD$1&amp;" "&amp;AD15,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ15" s="0" t="str">
         <f aca="false">IF(AE15="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE15))," --"&amp;AE$1&amp;" "&amp;AE15,""))</f>
@@ -16411,7 +16411,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
         <v>13</v>
       </c>
@@ -16426,7 +16426,7 @@
       </c>
       <c r="AH16" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B16,AI16,AJ16,AK16,AL16,AM16,AN16,AO16,AP16,AQ16,AR16,AS16,AT16,AU16,AV16,AW16,AX16,AY16,AZ16,BA16,BB16,BC16,BD16,BE16,BF16,BG16,BH16,BI16,BJ16,BK16,BL16)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH13 --standardize --zca --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH13 --standardize --zca --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI16" s="0" t="str">
         <f aca="false">IF(D16="y", " --"&amp;D$1,IF(NOT(ISBLANK(D16))," --"&amp;D$1&amp;" "&amp;D16,""))</f>
@@ -16534,7 +16534,7 @@
       </c>
       <c r="BI16" s="0" t="str">
         <f aca="false">IF(AD16="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD16))," --"&amp;AD$1&amp;" "&amp;AD16,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ16" s="0" t="str">
         <f aca="false">IF(AE16="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE16))," --"&amp;AE$1&amp;" "&amp;AE16,""))</f>
@@ -16545,7 +16545,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
         <v>14</v>
       </c>
@@ -16560,7 +16560,7 @@
       </c>
       <c r="AH17" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B17,AI17,AJ17,AK17,AL17,AM17,AN17,AO17,AP17,AQ17,AR17,AS17,AT17,AU17,AV17,AW17,AX17,AY17,AZ17,BA17,BB17,BC17,BD17,BE17,BF17,BG17,BH17,BI17,BJ17,BK17,BL17)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH14 --standardize --lecunlcn --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH14 --standardize --lecunlcn --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI17" s="0" t="str">
         <f aca="false">IF(D17="y", " --"&amp;D$1,IF(NOT(ISBLANK(D17))," --"&amp;D$1&amp;" "&amp;D17,""))</f>
@@ -16668,7 +16668,7 @@
       </c>
       <c r="BI17" s="0" t="str">
         <f aca="false">IF(AD17="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD17))," --"&amp;AD$1&amp;" "&amp;AD17,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ17" s="0" t="str">
         <f aca="false">IF(AE17="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE17))," --"&amp;AE$1&amp;" "&amp;AE17,""))</f>
@@ -16679,7 +16679,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
         <v>15</v>
       </c>
@@ -16697,7 +16697,7 @@
       </c>
       <c r="AH18" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B18,AI18,AJ18,AK18,AL18,AM18,AN18,AO18,AP18,AQ18,AR18,AS18,AT18,AU18,AV18,AW18,AX18,AY18,AZ18,BA18,BB18,BC18,BD18,BE18,BF18,BG18,BH18,BI18,BJ18,BK18,BL18)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH15 --standardize --zca --lecunlcn --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH15 --standardize --zca --lecunlcn --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI18" s="0" t="str">
         <f aca="false">IF(D18="y", " --"&amp;D$1,IF(NOT(ISBLANK(D18))," --"&amp;D$1&amp;" "&amp;D18,""))</f>
@@ -16805,7 +16805,7 @@
       </c>
       <c r="BI18" s="0" t="str">
         <f aca="false">IF(AD18="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD18))," --"&amp;AD$1&amp;" "&amp;AD18,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ18" s="0" t="str">
         <f aca="false">IF(AE18="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE18))," --"&amp;AE$1&amp;" "&amp;AE18,""))</f>
@@ -16816,7 +16816,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
         <v>16</v>
       </c>
@@ -16834,7 +16834,7 @@
       </c>
       <c r="AH19" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B19,AI19,AJ19,AK19,AL19,AM19,AN19,AO19,AP19,AQ19,AR19,AS19,AT19,AU19,AV19,AW19,AX19,AY19,AZ19,BA19,BB19,BC19,BD19,BE19,BF19,BG19,BH19,BI19,BJ19,BK19,BL19)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH16 --learningRate 0.01 --maxEpoch 300 --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH16 --learningRate 0.01 --maxEpoch 300 --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI19" s="0" t="str">
         <f aca="false">IF(D19="y", " --"&amp;D$1,IF(NOT(ISBLANK(D19))," --"&amp;D$1&amp;" "&amp;D19,""))</f>
@@ -16942,7 +16942,7 @@
       </c>
       <c r="BI19" s="0" t="str">
         <f aca="false">IF(AD19="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD19))," --"&amp;AD$1&amp;" "&amp;AD19,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ19" s="0" t="str">
         <f aca="false">IF(AE19="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE19))," --"&amp;AE$1&amp;" "&amp;AE19,""))</f>
@@ -16953,7 +16953,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
         <v>17</v>
       </c>
@@ -16971,7 +16971,7 @@
       </c>
       <c r="AH20" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B20,AI20,AJ20,AK20,AL20,AM20,AN20,AO20,AP20,AQ20,AR20,AS20,AT20,AU20,AV20,AW20,AX20,AY20,AZ20,BA20,BB20,BC20,BD20,BE20,BF20,BG20,BH20,BI20,BJ20,BK20,BL20)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH17 --learningRate 0.001 --maxEpoch 300 --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH17 --learningRate 0.001 --maxEpoch 300 --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI20" s="0" t="str">
         <f aca="false">IF(D20="y", " --"&amp;D$1,IF(NOT(ISBLANK(D20))," --"&amp;D$1&amp;" "&amp;D20,""))</f>
@@ -17079,7 +17079,7 @@
       </c>
       <c r="BI20" s="0" t="str">
         <f aca="false">IF(AD20="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD20))," --"&amp;AD$1&amp;" "&amp;AD20,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ20" s="0" t="str">
         <f aca="false">IF(AE20="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE20))," --"&amp;AE$1&amp;" "&amp;AE20,""))</f>
@@ -17090,7 +17090,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
         <v>18</v>
       </c>
@@ -17108,7 +17108,7 @@
       </c>
       <c r="AH21" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B21,AI21,AJ21,AK21,AL21,AM21,AN21,AO21,AP21,AQ21,AR21,AS21,AT21,AU21,AV21,AW21,AX21,AY21,AZ21,BA21,BB21,BC21,BD21,BE21,BF21,BG21,BH21,BI21,BJ21,BK21,BL21)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH18 --learningRate 0.0001 --maxEpoch 300 --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH18 --learningRate 0.0001 --maxEpoch 300 --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI21" s="0" t="str">
         <f aca="false">IF(D21="y", " --"&amp;D$1,IF(NOT(ISBLANK(D21))," --"&amp;D$1&amp;" "&amp;D21,""))</f>
@@ -17216,7 +17216,7 @@
       </c>
       <c r="BI21" s="0" t="str">
         <f aca="false">IF(AD21="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD21))," --"&amp;AD$1&amp;" "&amp;AD21,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ21" s="0" t="str">
         <f aca="false">IF(AE21="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE21))," --"&amp;AE$1&amp;" "&amp;AE21,""))</f>
@@ -17227,7 +17227,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="n">
         <v>19</v>
       </c>
@@ -17245,7 +17245,7 @@
       </c>
       <c r="AH22" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B22,AI22,AJ22,AK22,AL22,AM22,AN22,AO22,AP22,AQ22,AR22,AS22,AT22,AU22,AV22,AW22,AX22,AY22,AZ22,BA22,BB22,BC22,BD22,BE22,BF22,BG22,BH22,BI22,BJ22,BK22,BL22)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH19 --learningRate 0.1 --maxEpoch 300 --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH19 --learningRate 0.1 --maxEpoch 300 --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI22" s="0" t="str">
         <f aca="false">IF(D22="y", " --"&amp;D$1,IF(NOT(ISBLANK(D22))," --"&amp;D$1&amp;" "&amp;D22,""))</f>
@@ -17353,7 +17353,7 @@
       </c>
       <c r="BI22" s="0" t="str">
         <f aca="false">IF(AD22="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD22))," --"&amp;AD$1&amp;" "&amp;AD22,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ22" s="0" t="str">
         <f aca="false">IF(AE22="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE22))," --"&amp;AE$1&amp;" "&amp;AE22,""))</f>
@@ -17364,7 +17364,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="n">
         <v>20</v>
       </c>
@@ -17388,7 +17388,7 @@
       </c>
       <c r="AH23" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B23,AI23,AJ23,AK23,AL23,AM23,AN23,AO23,AP23,AQ23,AR23,AS23,AT23,AU23,AV23,AW23,AX23,AY23,AZ23,BA23,BB23,BC23,BD23,BE23,BF23,BG23,BH23,BI23,BJ23,BK23,BL23)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH20 --learningRate 0.001 --minLR 0.00000001 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH20 --learningRate 0.001 --minLR 0.00000001 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI23" s="0" t="str">
         <f aca="false">IF(D23="y", " --"&amp;D$1,IF(NOT(ISBLANK(D23))," --"&amp;D$1&amp;" "&amp;D23,""))</f>
@@ -17496,7 +17496,7 @@
       </c>
       <c r="BI23" s="0" t="str">
         <f aca="false">IF(AD23="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD23))," --"&amp;AD$1&amp;" "&amp;AD23,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ23" s="0" t="str">
         <f aca="false">IF(AE23="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE23))," --"&amp;AE$1&amp;" "&amp;AE23,""))</f>
@@ -17507,7 +17507,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="n">
         <v>21</v>
       </c>
@@ -17531,7 +17531,7 @@
       </c>
       <c r="AH24" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B24,AI24,AJ24,AK24,AL24,AM24,AN24,AO24,AP24,AQ24,AR24,AS24,AT24,AU24,AV24,AW24,AX24,AY24,AZ24,BA24,BB24,BC24,BD24,BE24,BF24,BG24,BH24,BI24,BJ24,BK24,BL24)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH21 --learningRate 0.001 --minLR 0.000000001 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH21 --learningRate 0.001 --minLR 0.000000001 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI24" s="0" t="str">
         <f aca="false">IF(D24="y", " --"&amp;D$1,IF(NOT(ISBLANK(D24))," --"&amp;D$1&amp;" "&amp;D24,""))</f>
@@ -17639,7 +17639,7 @@
       </c>
       <c r="BI24" s="0" t="str">
         <f aca="false">IF(AD24="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD24))," --"&amp;AD$1&amp;" "&amp;AD24,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ24" s="0" t="str">
         <f aca="false">IF(AE24="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE24))," --"&amp;AE$1&amp;" "&amp;AE24,""))</f>
@@ -17650,7 +17650,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="n">
         <v>22</v>
       </c>
@@ -17674,7 +17674,7 @@
       </c>
       <c r="AH25" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B25,AI25,AJ25,AK25,AL25,AM25,AN25,AO25,AP25,AQ25,AR25,AS25,AT25,AU25,AV25,AW25,AX25,AY25,AZ25,BA25,BB25,BC25,BD25,BE25,BF25,BG25,BH25,BI25,BJ25,BK25,BL25)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH22 --learningRate 0.001 --minLR 0.0000000001 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH22 --learningRate 0.001 --minLR 0.0000000001 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI25" s="0" t="str">
         <f aca="false">IF(D25="y", " --"&amp;D$1,IF(NOT(ISBLANK(D25))," --"&amp;D$1&amp;" "&amp;D25,""))</f>
@@ -17782,7 +17782,7 @@
       </c>
       <c r="BI25" s="0" t="str">
         <f aca="false">IF(AD25="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD25))," --"&amp;AD$1&amp;" "&amp;AD25,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ25" s="0" t="str">
         <f aca="false">IF(AE25="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE25))," --"&amp;AE$1&amp;" "&amp;AE25,""))</f>
@@ -17793,7 +17793,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="n">
         <v>23</v>
       </c>
@@ -17817,7 +17817,7 @@
       </c>
       <c r="AH26" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B26,AI26,AJ26,AK26,AL26,AM26,AN26,AO26,AP26,AQ26,AR26,AS26,AT26,AU26,AV26,AW26,AX26,AY26,AZ26,BA26,BB26,BC26,BD26,BE26,BF26,BG26,BH26,BI26,BJ26,BK26,BL26)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH23 --learningRate 0.001 --minLR 0.00000000001 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH23 --learningRate 0.001 --minLR 0.00000000001 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI26" s="0" t="str">
         <f aca="false">IF(D26="y", " --"&amp;D$1,IF(NOT(ISBLANK(D26))," --"&amp;D$1&amp;" "&amp;D26,""))</f>
@@ -17925,7 +17925,7 @@
       </c>
       <c r="BI26" s="0" t="str">
         <f aca="false">IF(AD26="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD26))," --"&amp;AD$1&amp;" "&amp;AD26,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ26" s="0" t="str">
         <f aca="false">IF(AE26="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE26))," --"&amp;AE$1&amp;" "&amp;AE26,""))</f>
@@ -17936,7 +17936,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="n">
         <v>24</v>
       </c>
@@ -17960,7 +17960,7 @@
       </c>
       <c r="AH27" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B27,AI27,AJ27,AK27,AL27,AM27,AN27,AO27,AP27,AQ27,AR27,AS27,AT27,AU27,AV27,AW27,AX27,AY27,AZ27,BA27,BB27,BC27,BD27,BE27,BF27,BG27,BH27,BI27,BJ27,BK27,BL27)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH24 --learningRate 0.001 --minLR 0.00000000001 --saturateEpoch 100 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH24 --learningRate 0.001 --minLR 0.00000000001 --saturateEpoch 100 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI27" s="0" t="str">
         <f aca="false">IF(D27="y", " --"&amp;D$1,IF(NOT(ISBLANK(D27))," --"&amp;D$1&amp;" "&amp;D27,""))</f>
@@ -18068,7 +18068,7 @@
       </c>
       <c r="BI27" s="0" t="str">
         <f aca="false">IF(AD27="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD27))," --"&amp;AD$1&amp;" "&amp;AD27,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ27" s="0" t="str">
         <f aca="false">IF(AE27="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE27))," --"&amp;AE$1&amp;" "&amp;AE27,""))</f>
@@ -18079,7 +18079,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="n">
         <v>25</v>
       </c>
@@ -18103,7 +18103,7 @@
       </c>
       <c r="AH28" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B28,AI28,AJ28,AK28,AL28,AM28,AN28,AO28,AP28,AQ28,AR28,AS28,AT28,AU28,AV28,AW28,AX28,AY28,AZ28,BA28,BB28,BC28,BD28,BE28,BF28,BG28,BH28,BI28,BJ28,BK28,BL28)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH25 --learningRate 0.1 --minLR 0.0000001 --saturateEpoch 100 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH25 --learningRate 0.1 --minLR 0.0000001 --saturateEpoch 100 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI28" s="0" t="str">
         <f aca="false">IF(D28="y", " --"&amp;D$1,IF(NOT(ISBLANK(D28))," --"&amp;D$1&amp;" "&amp;D28,""))</f>
@@ -18211,7 +18211,7 @@
       </c>
       <c r="BI28" s="0" t="str">
         <f aca="false">IF(AD28="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD28))," --"&amp;AD$1&amp;" "&amp;AD28,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ28" s="0" t="str">
         <f aca="false">IF(AE28="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE28))," --"&amp;AE$1&amp;" "&amp;AE28,""))</f>
@@ -18222,7 +18222,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="n">
         <v>26</v>
       </c>
@@ -18243,7 +18243,7 @@
       </c>
       <c r="AH29" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B29,AI29,AJ29,AK29,AL29,AM29,AN29,AO29,AP29,AQ29,AR29,AS29,AT29,AU29,AV29,AW29,AX29,AY29,AZ29,BA29,BB29,BC29,BD29,BE29,BF29,BG29,BH29,BI29,BJ29,BK29,BL29)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH26 --learningRate 0.01 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH26 --learningRate 0.01 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI29" s="0" t="str">
         <f aca="false">IF(D29="y", " --"&amp;D$1,IF(NOT(ISBLANK(D29))," --"&amp;D$1&amp;" "&amp;D29,""))</f>
@@ -18351,7 +18351,7 @@
       </c>
       <c r="BI29" s="0" t="str">
         <f aca="false">IF(AD29="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD29))," --"&amp;AD$1&amp;" "&amp;AD29,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ29" s="0" t="str">
         <f aca="false">IF(AE29="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE29))," --"&amp;AE$1&amp;" "&amp;AE29,""))</f>
@@ -18362,7 +18362,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="n">
         <v>27</v>
       </c>
@@ -18383,7 +18383,7 @@
       </c>
       <c r="AH30" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B30,AI30,AJ30,AK30,AL30,AM30,AN30,AO30,AP30,AQ30,AR30,AS30,AT30,AU30,AV30,AW30,AX30,AY30,AZ30,BA30,BB30,BC30,BD30,BE30,BF30,BG30,BH30,BI30,BJ30,BK30,BL30)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH27 --learningRate 0.001 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH27 --learningRate 0.001 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI30" s="0" t="str">
         <f aca="false">IF(D30="y", " --"&amp;D$1,IF(NOT(ISBLANK(D30))," --"&amp;D$1&amp;" "&amp;D30,""))</f>
@@ -18491,7 +18491,7 @@
       </c>
       <c r="BI30" s="0" t="str">
         <f aca="false">IF(AD30="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD30))," --"&amp;AD$1&amp;" "&amp;AD30,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ30" s="0" t="str">
         <f aca="false">IF(AE30="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE30))," --"&amp;AE$1&amp;" "&amp;AE30,""))</f>
@@ -18502,7 +18502,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="n">
         <v>28</v>
       </c>
@@ -18523,7 +18523,7 @@
       </c>
       <c r="AH31" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B31,AI31,AJ31,AK31,AL31,AM31,AN31,AO31,AP31,AQ31,AR31,AS31,AT31,AU31,AV31,AW31,AX31,AY31,AZ31,BA31,BB31,BC31,BD31,BE31,BF31,BG31,BH31,BI31,BJ31,BK31,BL31)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH28 --learningRate 0.0001 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH28 --learningRate 0.0001 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI31" s="0" t="str">
         <f aca="false">IF(D31="y", " --"&amp;D$1,IF(NOT(ISBLANK(D31))," --"&amp;D$1&amp;" "&amp;D31,""))</f>
@@ -18631,7 +18631,7 @@
       </c>
       <c r="BI31" s="0" t="str">
         <f aca="false">IF(AD31="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD31))," --"&amp;AD$1&amp;" "&amp;AD31,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ31" s="0" t="str">
         <f aca="false">IF(AE31="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE31))," --"&amp;AE$1&amp;" "&amp;AE31,""))</f>
@@ -18642,7 +18642,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="n">
         <v>29</v>
       </c>
@@ -18663,7 +18663,7 @@
       </c>
       <c r="AH32" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B32,AI32,AJ32,AK32,AL32,AM32,AN32,AO32,AP32,AQ32,AR32,AS32,AT32,AU32,AV32,AW32,AX32,AY32,AZ32,BA32,BB32,BC32,BD32,BE32,BF32,BG32,BH32,BI32,BJ32,BK32,BL32)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH29 --learningRate 0.1 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH29 --learningRate 0.1 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI32" s="0" t="str">
         <f aca="false">IF(D32="y", " --"&amp;D$1,IF(NOT(ISBLANK(D32))," --"&amp;D$1&amp;" "&amp;D32,""))</f>
@@ -18771,7 +18771,7 @@
       </c>
       <c r="BI32" s="0" t="str">
         <f aca="false">IF(AD32="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD32))," --"&amp;AD$1&amp;" "&amp;AD32,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ32" s="0" t="str">
         <f aca="false">IF(AE32="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE32))," --"&amp;AE$1&amp;" "&amp;AE32,""))</f>
@@ -18782,7 +18782,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
         <v>30</v>
       </c>
@@ -18806,7 +18806,7 @@
       </c>
       <c r="AH33" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B33,AI33,AJ33,AK33,AL33,AM33,AN33,AO33,AP33,AQ33,AR33,AS33,AT33,AU33,AV33,AW33,AX33,AY33,AZ33,BA33,BB33,BC33,BD33,BE33,BF33,BG33,BH33,BI33,BJ33,BK33,BL33)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH30 --learningRate 0.001 --minLR 0.0000001 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH30 --learningRate 0.001 --minLR 0.0000001 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI33" s="0" t="str">
         <f aca="false">IF(D33="y", " --"&amp;D$1,IF(NOT(ISBLANK(D33))," --"&amp;D$1&amp;" "&amp;D33,""))</f>
@@ -18914,7 +18914,7 @@
       </c>
       <c r="BI33" s="0" t="str">
         <f aca="false">IF(AD33="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD33))," --"&amp;AD$1&amp;" "&amp;AD33,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ33" s="0" t="str">
         <f aca="false">IF(AE33="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE33))," --"&amp;AE$1&amp;" "&amp;AE33,""))</f>
@@ -18925,7 +18925,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="n">
         <v>31</v>
       </c>
@@ -18949,7 +18949,7 @@
       </c>
       <c r="AH34" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B34,AI34,AJ34,AK34,AL34,AM34,AN34,AO34,AP34,AQ34,AR34,AS34,AT34,AU34,AV34,AW34,AX34,AY34,AZ34,BA34,BB34,BC34,BD34,BE34,BF34,BG34,BH34,BI34,BJ34,BK34,BL34)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH31 --learningRate 0.001 --momentum 1 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH31 --learningRate 0.001 --momentum 1 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI34" s="0" t="str">
         <f aca="false">IF(D34="y", " --"&amp;D$1,IF(NOT(ISBLANK(D34))," --"&amp;D$1&amp;" "&amp;D34,""))</f>
@@ -19057,7 +19057,7 @@
       </c>
       <c r="BI34" s="0" t="str">
         <f aca="false">IF(AD34="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD34))," --"&amp;AD$1&amp;" "&amp;AD34,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ34" s="0" t="str">
         <f aca="false">IF(AE34="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE34))," --"&amp;AE$1&amp;" "&amp;AE34,""))</f>
@@ -19068,7 +19068,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="n">
         <v>32</v>
       </c>
@@ -19092,7 +19092,7 @@
       </c>
       <c r="AH35" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B35,AI35,AJ35,AK35,AL35,AM35,AN35,AO35,AP35,AQ35,AR35,AS35,AT35,AU35,AV35,AW35,AX35,AY35,AZ35,BA35,BB35,BC35,BD35,BE35,BF35,BG35,BH35,BI35,BJ35,BK35,BL35)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH32 --learningRate 0.001 --maxEpoch 300 --standardize --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH32 --learningRate 0.001 --maxEpoch 300 --standardize --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI35" s="0" t="str">
         <f aca="false">IF(D35="y", " --"&amp;D$1,IF(NOT(ISBLANK(D35))," --"&amp;D$1&amp;" "&amp;D35,""))</f>
@@ -19200,7 +19200,7 @@
       </c>
       <c r="BI35" s="0" t="str">
         <f aca="false">IF(AD35="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD35))," --"&amp;AD$1&amp;" "&amp;AD35,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ35" s="0" t="str">
         <f aca="false">IF(AE35="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE35))," --"&amp;AE$1&amp;" "&amp;AE35,""))</f>
@@ -19211,7 +19211,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="n">
         <v>33</v>
       </c>
@@ -19235,7 +19235,7 @@
       </c>
       <c r="AH36" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B36,AI36,AJ36,AK36,AL36,AM36,AN36,AO36,AP36,AQ36,AR36,AS36,AT36,AU36,AV36,AW36,AX36,AY36,AZ36,BA36,BB36,BC36,BD36,BE36,BF36,BG36,BH36,BI36,BJ36,BK36,BL36)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH33 --learningRate 0.001 --maxEpoch 300 --zca --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH33 --learningRate 0.001 --maxEpoch 300 --zca --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI36" s="0" t="str">
         <f aca="false">IF(D36="y", " --"&amp;D$1,IF(NOT(ISBLANK(D36))," --"&amp;D$1&amp;" "&amp;D36,""))</f>
@@ -19343,7 +19343,7 @@
       </c>
       <c r="BI36" s="0" t="str">
         <f aca="false">IF(AD36="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD36))," --"&amp;AD$1&amp;" "&amp;AD36,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ36" s="0" t="str">
         <f aca="false">IF(AE36="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE36))," --"&amp;AE$1&amp;" "&amp;AE36,""))</f>
@@ -19354,7 +19354,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="n">
         <v>34</v>
       </c>
@@ -19378,7 +19378,7 @@
       </c>
       <c r="AH37" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B37,AI37,AJ37,AK37,AL37,AM37,AN37,AO37,AP37,AQ37,AR37,AS37,AT37,AU37,AV37,AW37,AX37,AY37,AZ37,BA37,BB37,BC37,BD37,BE37,BF37,BG37,BH37,BI37,BJ37,BK37,BL37)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH34 --learningRate 0.001 --maxEpoch 300 --lecunlcn --activation ReLU --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH34 --learningRate 0.001 --maxEpoch 300 --lecunlcn --activation ReLU --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI37" s="0" t="str">
         <f aca="false">IF(D37="y", " --"&amp;D$1,IF(NOT(ISBLANK(D37))," --"&amp;D$1&amp;" "&amp;D37,""))</f>
@@ -19486,7 +19486,7 @@
       </c>
       <c r="BI37" s="0" t="str">
         <f aca="false">IF(AD37="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD37))," --"&amp;AD$1&amp;" "&amp;AD37,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ37" s="0" t="str">
         <f aca="false">IF(AE37="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE37))," --"&amp;AE$1&amp;" "&amp;AE37,""))</f>
@@ -19497,7 +19497,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="n">
         <v>35</v>
       </c>
@@ -19521,7 +19521,7 @@
       </c>
       <c r="AH38" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B38,AI38,AJ38,AK38,AL38,AM38,AN38,AO38,AP38,AQ38,AR38,AS38,AT38,AU38,AV38,AW38,AX38,AY38,AZ38,BA38,BB38,BC38,BD38,BE38,BF38,BG38,BH38,BI38,BJ38,BK38,BL38)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH35 --learningRate 0.001 --maxEpoch 300 --lecunlcn --activation Sigmoid --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH35 --learningRate 0.001 --maxEpoch 300 --lecunlcn --activation Sigmoid --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI38" s="0" t="str">
         <f aca="false">IF(D38="y", " --"&amp;D$1,IF(NOT(ISBLANK(D38))," --"&amp;D$1&amp;" "&amp;D38,""))</f>
@@ -19629,7 +19629,7 @@
       </c>
       <c r="BI38" s="0" t="str">
         <f aca="false">IF(AD38="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD38))," --"&amp;AD$1&amp;" "&amp;AD38,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ38" s="0" t="str">
         <f aca="false">IF(AE38="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE38))," --"&amp;AE$1&amp;" "&amp;AE38,""))</f>
@@ -19640,7 +19640,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="n">
         <v>36</v>
       </c>
@@ -19661,7 +19661,7 @@
       </c>
       <c r="AH39" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B39,AI39,AJ39,AK39,AL39,AM39,AN39,AO39,AP39,AQ39,AR39,AS39,AT39,AU39,AV39,AW39,AX39,AY39,AZ39,BA39,BB39,BC39,BD39,BE39,BF39,BG39,BH39,BI39,BJ39,BK39,BL39)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH36 --learningRate 0.001 --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000) --dropout</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH36 --learningRate 0.001 --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’ --dropout</v>
       </c>
       <c r="AI39" s="0" t="str">
         <f aca="false">IF(D39="y", " --"&amp;D$1,IF(NOT(ISBLANK(D39))," --"&amp;D$1&amp;" "&amp;D39,""))</f>
@@ -19769,7 +19769,7 @@
       </c>
       <c r="BI39" s="0" t="str">
         <f aca="false">IF(AD39="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD39))," --"&amp;AD$1&amp;" "&amp;AD39,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ39" s="0" t="str">
         <f aca="false">IF(AE39="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE39))," --"&amp;AE$1&amp;" "&amp;AE39,""))</f>
@@ -19780,7 +19780,7 @@
         <v> --dropout</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="n">
         <v>37</v>
       </c>
@@ -19801,7 +19801,7 @@
       </c>
       <c r="AH40" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B40,AI40,AJ40,AK40,AL40,AM40,AN40,AO40,AP40,AQ40,AR40,AS40,AT40,AU40,AV40,AW40,AX40,AY40,AZ40,BA40,BB40,BC40,BD40,BE40,BF40,BG40,BH40,BI40,BJ40,BK40,BL40)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH37 --learningRate 0.001 --padding --maxEpoch 300 --lecunlcn --hiddenSize {4000,4000)</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH37 --learningRate 0.001 --padding --maxEpoch 300 --lecunlcn --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="AI40" s="0" t="str">
         <f aca="false">IF(D40="y", " --"&amp;D$1,IF(NOT(ISBLANK(D40))," --"&amp;D$1&amp;" "&amp;D40,""))</f>
@@ -19909,7 +19909,7 @@
       </c>
       <c r="BI40" s="0" t="str">
         <f aca="false">IF(AD40="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD40))," --"&amp;AD$1&amp;" "&amp;AD40,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ40" s="0" t="str">
         <f aca="false">IF(AE40="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE40))," --"&amp;AE$1&amp;" "&amp;AE40,""))</f>
@@ -19920,7 +19920,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="n">
         <v>38</v>
       </c>
@@ -19944,7 +19944,7 @@
       </c>
       <c r="AH41" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B41,AI41,AJ41,AK41,AL41,AM41,AN41,AO41,AP41,AQ41,AR41,AS41,AT41,AU41,AV41,AW41,AX41,AY41,AZ41,BA41,BB41,BC41,BD41,BE41,BF41,BG41,BH41,BI41,BJ41,BK41,BL41)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH38 --learningRate 0.001 --minLR 0.0000001 --lecunlcn --activation ReLU --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH38 --learningRate 0.001 --minLR 0.0000001 --lecunlcn --activation ReLU --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI41" s="0" t="str">
         <f aca="false">IF(D41="y", " --"&amp;D$1,IF(NOT(ISBLANK(D41))," --"&amp;D$1&amp;" "&amp;D41,""))</f>
@@ -20052,7 +20052,7 @@
       </c>
       <c r="BI41" s="0" t="str">
         <f aca="false">IF(AD41="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD41))," --"&amp;AD$1&amp;" "&amp;AD41,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ41" s="0" t="str">
         <f aca="false">IF(AE41="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE41))," --"&amp;AE$1&amp;" "&amp;AE41,""))</f>
@@ -20063,7 +20063,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="n">
         <v>39</v>
       </c>
@@ -20087,7 +20087,7 @@
       </c>
       <c r="AH42" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B42,AI42,AJ42,AK42,AL42,AM42,AN42,AO42,AP42,AQ42,AR42,AS42,AT42,AU42,AV42,AW42,AX42,AY42,AZ42,BA42,BB42,BC42,BD42,BE42,BF42,BG42,BH42,BI42,BJ42,BK42,BL42)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH39 --learningRate 0.001 --minLR 0.0000001 --zca --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH39 --learningRate 0.001 --minLR 0.0000001 --zca --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI42" s="0" t="str">
         <f aca="false">IF(D42="y", " --"&amp;D$1,IF(NOT(ISBLANK(D42))," --"&amp;D$1&amp;" "&amp;D42,""))</f>
@@ -20195,7 +20195,7 @@
       </c>
       <c r="BI42" s="0" t="str">
         <f aca="false">IF(AD42="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD42))," --"&amp;AD$1&amp;" "&amp;AD42,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ42" s="0" t="str">
         <f aca="false">IF(AE42="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE42))," --"&amp;AE$1&amp;" "&amp;AE42,""))</f>
@@ -20206,7 +20206,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="n">
         <v>40</v>
       </c>
@@ -20230,7 +20230,7 @@
       </c>
       <c r="AH43" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B43,AI43,AJ43,AK43,AL43,AM43,AN43,AO43,AP43,AQ43,AR43,AS43,AT43,AU43,AV43,AW43,AX43,AY43,AZ43,BA43,BB43,BC43,BD43,BE43,BF43,BG43,BH43,BI43,BJ43,BK43,BL43)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH40 --learningRate 0.001 --minLR 0.0000001 --standardize --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH40 --learningRate 0.001 --minLR 0.0000001 --standardize --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI43" s="0" t="str">
         <f aca="false">IF(D43="y", " --"&amp;D$1,IF(NOT(ISBLANK(D43))," --"&amp;D$1&amp;" "&amp;D43,""))</f>
@@ -20338,7 +20338,7 @@
       </c>
       <c r="BI43" s="0" t="str">
         <f aca="false">IF(AD43="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD43))," --"&amp;AD$1&amp;" "&amp;AD43,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ43" s="0" t="str">
         <f aca="false">IF(AE43="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE43))," --"&amp;AE$1&amp;" "&amp;AE43,""))</f>
@@ -20349,7 +20349,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="n">
         <v>41</v>
       </c>
@@ -20376,7 +20376,7 @@
       </c>
       <c r="AH44" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B44,AI44,AJ44,AK44,AL44,AM44,AN44,AO44,AP44,AQ44,AR44,AS44,AT44,AU44,AV44,AW44,AX44,AY44,AZ44,BA44,BB44,BC44,BD44,BE44,BF44,BG44,BH44,BI44,BJ44,BK44,BL44)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH41 --learningRate 0.001 --minLR 0.00000000001 --saturateEpoch 100 --standardize --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH41 --learningRate 0.001 --minLR 0.00000000001 --saturateEpoch 100 --standardize --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI44" s="0" t="str">
         <f aca="false">IF(D44="y", " --"&amp;D$1,IF(NOT(ISBLANK(D44))," --"&amp;D$1&amp;" "&amp;D44,""))</f>
@@ -20484,7 +20484,7 @@
       </c>
       <c r="BI44" s="0" t="str">
         <f aca="false">IF(AD44="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD44))," --"&amp;AD$1&amp;" "&amp;AD44,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ44" s="0" t="str">
         <f aca="false">IF(AE44="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE44))," --"&amp;AE$1&amp;" "&amp;AE44,""))</f>
@@ -20495,7 +20495,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="n">
         <v>42</v>
       </c>
@@ -20519,7 +20519,7 @@
       </c>
       <c r="AH45" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B45,AI45,AJ45,AK45,AL45,AM45,AN45,AO45,AP45,AQ45,AR45,AS45,AT45,AU45,AV45,AW45,AX45,AY45,AZ45,BA45,BB45,BC45,BD45,BE45,BF45,BG45,BH45,BI45,BJ45,BK45,BL45)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH42 --learningRate 0.001 --minLR 0.0000001 --batchSize 96 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH42 --learningRate 0.001 --minLR 0.0000001 --batchSize 96 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI45" s="0" t="str">
         <f aca="false">IF(D45="y", " --"&amp;D$1,IF(NOT(ISBLANK(D45))," --"&amp;D$1&amp;" "&amp;D45,""))</f>
@@ -20627,7 +20627,7 @@
       </c>
       <c r="BI45" s="0" t="str">
         <f aca="false">IF(AD45="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD45))," --"&amp;AD$1&amp;" "&amp;AD45,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ45" s="0" t="str">
         <f aca="false">IF(AE45="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE45))," --"&amp;AE$1&amp;" "&amp;AE45,""))</f>
@@ -20638,7 +20638,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="n">
         <v>43</v>
       </c>
@@ -20662,7 +20662,7 @@
       </c>
       <c r="AH46" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B46,AI46,AJ46,AK46,AL46,AM46,AN46,AO46,AP46,AQ46,AR46,AS46,AT46,AU46,AV46,AW46,AX46,AY46,AZ46,BA46,BB46,BC46,BD46,BE46,BF46,BG46,BH46,BI46,BJ46,BK46,BL46)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH43 --learningRate 0.001 --minLR 0.0000001 --batchSize 128 --lecunlcn --hiddenSize {4000,4000) --batchNorm</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH43 --learningRate 0.001 --minLR 0.0000001 --batchSize 128 --lecunlcn --hiddenSize ‘{4000,4000}’ --batchNorm</v>
       </c>
       <c r="AI46" s="0" t="str">
         <f aca="false">IF(D46="y", " --"&amp;D$1,IF(NOT(ISBLANK(D46))," --"&amp;D$1&amp;" "&amp;D46,""))</f>
@@ -20770,7 +20770,7 @@
       </c>
       <c r="BI46" s="0" t="str">
         <f aca="false">IF(AD46="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD46))," --"&amp;AD$1&amp;" "&amp;AD46,""))</f>
-        <v> --hiddenSize {4000,4000)</v>
+        <v> --hiddenSize ‘{4000,4000}’</v>
       </c>
       <c r="BJ46" s="0" t="str">
         <f aca="false">IF(AE46="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE46))," --"&amp;AE$1&amp;" "&amp;AE46,""))</f>

</xml_diff>

<commit_message>
several smaller conv experiments
</commit_message>
<xml_diff>
--- a/convParameters.xlsx
+++ b/convParameters.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="123">
   <si>
     <t xml:space="preserve">Experiemnt Prefix</t>
   </si>
@@ -250,7 +250,13 @@
     <t xml:space="preserve">‘{4000,4000}’</t>
   </si>
   <si>
-    <t xml:space="preserve">‘{400}’</t>
+    <t xml:space="preserve"> '{400}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'{10746,4000}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'{40,40}'</t>
   </si>
   <si>
     <t xml:space="preserve">dontPad</t>
@@ -502,9 +508,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="34" min="1" style="0" width="9.80566801619433"/>
-    <col collapsed="false" hidden="false" max="64" min="35" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="65" style="0" width="9.80566801619433"/>
+    <col collapsed="false" hidden="false" max="34" min="1" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="64" min="35" style="0" width="11.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1025" min="65" style="0" width="10.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13854,8 +13860,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="4.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8178137651822"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14395,15 +14400,15 @@
   </sheetPr>
   <dimension ref="A1:BK103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB44" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD50" activeCellId="0" sqref="AD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="33" min="1" style="0" width="9.80566801619433"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="179.696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="9.80566801619433"/>
+    <col collapsed="false" hidden="false" max="33" min="1" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="191.421052631579"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="10.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20814,11 +20819,11 @@
       </c>
       <c r="AH47" s="0" t="str">
         <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B47,AI47,AJ47,AK47,AL47,AM47,AN47,AO47,AP47,AQ47,AR47,AS47,AT47,AU47,AV47,AW47,AX47,AY47,AZ47,BA47,BB47,BC47,BD47,BE47,BF47,BG47,BH47,BI47,BJ47,BK47,BL47)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH44 --learningRate 0.001 --minLR 0.0000001 --standardize --zca --lecunlcn --hiddenSize ‘{400}’ --batchNorm --dropout</v>
+        <v>docker exec -it $IMAGE ./convExperiment.sh EH44--learningRate 0.001--minLR 0.0000001--standardize--zca--lecunlcn --hiddenSize  '{400}'--batchNorm--dropout</v>
       </c>
       <c r="AI47" s="0" t="str">
         <f aca="false">IF(D47="y", " --"&amp;D$1,IF(NOT(ISBLANK(D47))," --"&amp;D$1&amp;" "&amp;D47,""))</f>
-        <v> --learningRate 0.001</v>
+        <v>--learningRate 0.001</v>
       </c>
       <c r="AJ47" s="0" t="str">
         <f aca="false">IF(E47="y", " --"&amp;E$1,IF(NOT(ISBLANK(E47))," --"&amp;E$1&amp;" "&amp;E47,""))</f>
@@ -20826,7 +20831,7 @@
       </c>
       <c r="AK47" s="0" t="str">
         <f aca="false">IF(F47="y", " --"&amp;F$1,IF(NOT(ISBLANK(F47))," --"&amp;F$1&amp;" "&amp;F47,""))</f>
-        <v> --minLR 0.0000001</v>
+        <v>--minLR 0.0000001</v>
       </c>
       <c r="AL47" s="0" t="str">
         <f aca="false">IF(G47="y", " --"&amp;G$1,IF(NOT(ISBLANK(G47))," --"&amp;G$1&amp;" "&amp;G47,""))</f>
@@ -20906,15 +20911,15 @@
       </c>
       <c r="BE47" s="0" t="str">
         <f aca="false">IF(Z47="y", " --"&amp;Z$1,IF(NOT(ISBLANK(Z47))," --"&amp;Z$1&amp;" "&amp;Z47,""))</f>
-        <v> --standardize</v>
+        <v>--standardize</v>
       </c>
       <c r="BF47" s="0" t="str">
         <f aca="false">IF(AA47="y", " --"&amp;AA$1,IF(NOT(ISBLANK(AA47))," --"&amp;AA$1&amp;" "&amp;AA47,""))</f>
-        <v> --zca</v>
+        <v>--zca</v>
       </c>
       <c r="BG47" s="0" t="str">
         <f aca="false">IF(AB47="y", " --"&amp;AB$1,IF(NOT(ISBLANK(AB47))," --"&amp;AB$1&amp;" "&amp;AB47,""))</f>
-        <v> --lecunlcn</v>
+        <v>--lecunlcn</v>
       </c>
       <c r="BH47" s="0" t="str">
         <f aca="false">IF(AC47="y", " --"&amp;AC$1,IF(NOT(ISBLANK(AC47))," --"&amp;AC$1&amp;" "&amp;AC47,""))</f>
@@ -20922,28 +20927,52 @@
       </c>
       <c r="BI47" s="0" t="str">
         <f aca="false">IF(AD47="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD47))," --"&amp;AD$1&amp;" "&amp;AD47,""))</f>
-        <v> --hiddenSize ‘{400}’</v>
+        <v> --hiddenSize  '{400}'</v>
       </c>
       <c r="BJ47" s="0" t="str">
         <f aca="false">IF(AE47="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE47))," --"&amp;AE$1&amp;" "&amp;AE47,""))</f>
-        <v> --batchNorm</v>
+        <v>--batchNorm</v>
       </c>
       <c r="BK47" s="0" t="str">
         <f aca="false">IF(AF47="y", " --"&amp;AF$1,IF(NOT(ISBLANK(AF47))," --"&amp;AF$1&amp;" "&amp;AF47,""))</f>
-        <v> --dropout</v>
+        <v>--dropout</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="D48" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F48" s="2" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="Z48" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA48" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB48" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD48" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE48" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF48" s="0" t="s">
+        <v>68</v>
+      </c>
       <c r="AH48" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B48,AI48,AJ48,AK48,AL48,AM48,AN48,AO48,AP48,AQ48,AR48,AS48,AT48,AU48,AV48,AW48,AX48,AY48,AZ48,BA48,BB48,BC48,BD48,BE48,BF48,BG48,BH48,BI48,BJ48,BK48,BL48)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH45</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,"_2_",B48,AI48,AJ48,AK48,AL48,AM48,AN48,AO48,AP48,AQ48,AR48,AS48,AT48,AU48,AV48,AW48,AX48,AY48,AZ48,BA48,BB48,BC48,BD48,BE48,BF48,BG48,BH48,BI48,BJ48,BK48,BL48)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH_2_45 --learningRate 0.001 --minLR 0.0000001 --standardize --zca --lecunlcn --hiddenSize '{10746,4000}' --batchNorm --dropout</v>
       </c>
       <c r="AI48" s="0" t="str">
         <f aca="false">IF(D48="y", " --"&amp;D$1,IF(NOT(ISBLANK(D48))," --"&amp;D$1&amp;" "&amp;D48,""))</f>
-        <v/>
+        <v> --learningRate 0.001</v>
       </c>
       <c r="AJ48" s="0" t="str">
         <f aca="false">IF(E48="y", " --"&amp;E$1,IF(NOT(ISBLANK(E48))," --"&amp;E$1&amp;" "&amp;E48,""))</f>
@@ -20951,7 +20980,7 @@
       </c>
       <c r="AK48" s="0" t="str">
         <f aca="false">IF(F48="y", " --"&amp;F$1,IF(NOT(ISBLANK(F48))," --"&amp;F$1&amp;" "&amp;F48,""))</f>
-        <v/>
+        <v> --minLR 0.0000001</v>
       </c>
       <c r="AL48" s="0" t="str">
         <f aca="false">IF(G48="y", " --"&amp;G$1,IF(NOT(ISBLANK(G48))," --"&amp;G$1&amp;" "&amp;G48,""))</f>
@@ -21031,15 +21060,15 @@
       </c>
       <c r="BE48" s="0" t="str">
         <f aca="false">IF(Z48="y", " --"&amp;Z$1,IF(NOT(ISBLANK(Z48))," --"&amp;Z$1&amp;" "&amp;Z48,""))</f>
-        <v/>
+        <v> --standardize</v>
       </c>
       <c r="BF48" s="0" t="str">
         <f aca="false">IF(AA48="y", " --"&amp;AA$1,IF(NOT(ISBLANK(AA48))," --"&amp;AA$1&amp;" "&amp;AA48,""))</f>
-        <v/>
+        <v> --zca</v>
       </c>
       <c r="BG48" s="0" t="str">
         <f aca="false">IF(AB48="y", " --"&amp;AB$1,IF(NOT(ISBLANK(AB48))," --"&amp;AB$1&amp;" "&amp;AB48,""))</f>
-        <v/>
+        <v> --lecunlcn</v>
       </c>
       <c r="BH48" s="0" t="str">
         <f aca="false">IF(AC48="y", " --"&amp;AC$1,IF(NOT(ISBLANK(AC48))," --"&amp;AC$1&amp;" "&amp;AC48,""))</f>
@@ -21047,28 +21076,49 @@
       </c>
       <c r="BI48" s="0" t="str">
         <f aca="false">IF(AD48="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD48))," --"&amp;AD$1&amp;" "&amp;AD48,""))</f>
-        <v/>
+        <v> --hiddenSize '{10746,4000}'</v>
       </c>
       <c r="BJ48" s="0" t="str">
         <f aca="false">IF(AE48="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE48))," --"&amp;AE$1&amp;" "&amp;AE48,""))</f>
-        <v/>
+        <v> --batchNorm</v>
       </c>
       <c r="BK48" s="0" t="str">
         <f aca="false">IF(AF48="y", " --"&amp;AF$1,IF(NOT(ISBLANK(AF48))," --"&amp;AF$1&amp;" "&amp;AF48,""))</f>
-        <v/>
+        <v> --dropout</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="n">
         <v>46</v>
       </c>
+      <c r="D49" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F49" s="2" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="Z49" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA49" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB49" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE49" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF49" s="0" t="s">
+        <v>68</v>
+      </c>
       <c r="AH49" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B49,AI49,AJ49,AK49,AL49,AM49,AN49,AO49,AP49,AQ49,AR49,AS49,AT49,AU49,AV49,AW49,AX49,AY49,AZ49,BA49,BB49,BC49,BD49,BE49,BF49,BG49,BH49,BI49,BJ49,BK49,BL49)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH46</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,"_2_",B49,AI49,AJ49,AK49,AL49,AM49,AN49,AO49,AP49,AQ49,AR49,AS49,AT49,AU49,AV49,AW49,AX49,AY49,AZ49,BA49,BB49,BC49,BD49,BE49,BF49,BG49,BH49,BI49,BJ49,BK49,BL49)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH_2_46 --learningRate 0.001 --minLR 0.0000001 --standardize --zca --lecunlcn --batchNorm --dropout</v>
       </c>
       <c r="AI49" s="0" t="str">
         <f aca="false">IF(D49="y", " --"&amp;D$1,IF(NOT(ISBLANK(D49))," --"&amp;D$1&amp;" "&amp;D49,""))</f>
-        <v/>
+        <v> --learningRate 0.001</v>
       </c>
       <c r="AJ49" s="0" t="str">
         <f aca="false">IF(E49="y", " --"&amp;E$1,IF(NOT(ISBLANK(E49))," --"&amp;E$1&amp;" "&amp;E49,""))</f>
@@ -21076,7 +21126,7 @@
       </c>
       <c r="AK49" s="0" t="str">
         <f aca="false">IF(F49="y", " --"&amp;F$1,IF(NOT(ISBLANK(F49))," --"&amp;F$1&amp;" "&amp;F49,""))</f>
-        <v/>
+        <v> --minLR 0.0000001</v>
       </c>
       <c r="AL49" s="0" t="str">
         <f aca="false">IF(G49="y", " --"&amp;G$1,IF(NOT(ISBLANK(G49))," --"&amp;G$1&amp;" "&amp;G49,""))</f>
@@ -21156,15 +21206,15 @@
       </c>
       <c r="BE49" s="0" t="str">
         <f aca="false">IF(Z49="y", " --"&amp;Z$1,IF(NOT(ISBLANK(Z49))," --"&amp;Z$1&amp;" "&amp;Z49,""))</f>
-        <v/>
+        <v> --standardize</v>
       </c>
       <c r="BF49" s="0" t="str">
         <f aca="false">IF(AA49="y", " --"&amp;AA$1,IF(NOT(ISBLANK(AA49))," --"&amp;AA$1&amp;" "&amp;AA49,""))</f>
-        <v/>
+        <v> --zca</v>
       </c>
       <c r="BG49" s="0" t="str">
         <f aca="false">IF(AB49="y", " --"&amp;AB$1,IF(NOT(ISBLANK(AB49))," --"&amp;AB$1&amp;" "&amp;AB49,""))</f>
-        <v/>
+        <v> --lecunlcn</v>
       </c>
       <c r="BH49" s="0" t="str">
         <f aca="false">IF(AC49="y", " --"&amp;AC$1,IF(NOT(ISBLANK(AC49))," --"&amp;AC$1&amp;" "&amp;AC49,""))</f>
@@ -21176,24 +21226,48 @@
       </c>
       <c r="BJ49" s="0" t="str">
         <f aca="false">IF(AE49="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE49))," --"&amp;AE$1&amp;" "&amp;AE49,""))</f>
-        <v/>
+        <v> --batchNorm</v>
       </c>
       <c r="BK49" s="0" t="str">
         <f aca="false">IF(AF49="y", " --"&amp;AF$1,IF(NOT(ISBLANK(AF49))," --"&amp;AF$1&amp;" "&amp;AF49,""))</f>
-        <v/>
+        <v> --dropout</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="n">
         <v>47</v>
       </c>
+      <c r="D50" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F50" s="2" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="Z50" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA50" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB50" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD50" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE50" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF50" s="0" t="s">
+        <v>68</v>
+      </c>
       <c r="AH50" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B50,AI50,AJ50,AK50,AL50,AM50,AN50,AO50,AP50,AQ50,AR50,AS50,AT50,AU50,AV50,AW50,AX50,AY50,AZ50,BA50,BB50,BC50,BD50,BE50,BF50,BG50,BH50,BI50,BJ50,BK50,BL50)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH47</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,"_2_",B50,AI50,AJ50,AK50,AL50,AM50,AN50,AO50,AP50,AQ50,AR50,AS50,AT50,AU50,AV50,AW50,AX50,AY50,AZ50,BA50,BB50,BC50,BD50,BE50,BF50,BG50,BH50,BI50,BJ50,BK50,BL50)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH_2_47 --learningRate 0.001 --minLR 0.0000001 --standardize --zca --lecunlcn --hiddenSize '{40,40}' --batchNorm --dropout</v>
       </c>
       <c r="AI50" s="0" t="str">
         <f aca="false">IF(D50="y", " --"&amp;D$1,IF(NOT(ISBLANK(D50))," --"&amp;D$1&amp;" "&amp;D50,""))</f>
-        <v/>
+        <v> --learningRate 0.001</v>
       </c>
       <c r="AJ50" s="0" t="str">
         <f aca="false">IF(E50="y", " --"&amp;E$1,IF(NOT(ISBLANK(E50))," --"&amp;E$1&amp;" "&amp;E50,""))</f>
@@ -21201,7 +21275,7 @@
       </c>
       <c r="AK50" s="0" t="str">
         <f aca="false">IF(F50="y", " --"&amp;F$1,IF(NOT(ISBLANK(F50))," --"&amp;F$1&amp;" "&amp;F50,""))</f>
-        <v/>
+        <v> --minLR 0.0000001</v>
       </c>
       <c r="AL50" s="0" t="str">
         <f aca="false">IF(G50="y", " --"&amp;G$1,IF(NOT(ISBLANK(G50))," --"&amp;G$1&amp;" "&amp;G50,""))</f>
@@ -21281,15 +21355,15 @@
       </c>
       <c r="BE50" s="0" t="str">
         <f aca="false">IF(Z50="y", " --"&amp;Z$1,IF(NOT(ISBLANK(Z50))," --"&amp;Z$1&amp;" "&amp;Z50,""))</f>
-        <v/>
+        <v> --standardize</v>
       </c>
       <c r="BF50" s="0" t="str">
         <f aca="false">IF(AA50="y", " --"&amp;AA$1,IF(NOT(ISBLANK(AA50))," --"&amp;AA$1&amp;" "&amp;AA50,""))</f>
-        <v/>
+        <v> --zca</v>
       </c>
       <c r="BG50" s="0" t="str">
         <f aca="false">IF(AB50="y", " --"&amp;AB$1,IF(NOT(ISBLANK(AB50))," --"&amp;AB$1&amp;" "&amp;AB50,""))</f>
-        <v/>
+        <v> --lecunlcn</v>
       </c>
       <c r="BH50" s="0" t="str">
         <f aca="false">IF(AC50="y", " --"&amp;AC$1,IF(NOT(ISBLANK(AC50))," --"&amp;AC$1&amp;" "&amp;AC50,""))</f>
@@ -21297,24 +21371,25 @@
       </c>
       <c r="BI50" s="0" t="str">
         <f aca="false">IF(AD50="y", " --"&amp;AD$1,IF(NOT(ISBLANK(AD50))," --"&amp;AD$1&amp;" "&amp;AD50,""))</f>
-        <v/>
+        <v> --hiddenSize '{40,40}'</v>
       </c>
       <c r="BJ50" s="0" t="str">
         <f aca="false">IF(AE50="y", " --"&amp;AE$1,IF(NOT(ISBLANK(AE50))," --"&amp;AE$1&amp;" "&amp;AE50,""))</f>
-        <v/>
+        <v> --batchNorm</v>
       </c>
       <c r="BK50" s="0" t="str">
         <f aca="false">IF(AF50="y", " --"&amp;AF$1,IF(NOT(ISBLANK(AF50))," --"&amp;AF$1&amp;" "&amp;AF50,""))</f>
-        <v/>
+        <v> --dropout</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="F51" s="2"/>
       <c r="AH51" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B51,AI51,AJ51,AK51,AL51,AM51,AN51,AO51,AP51,AQ51,AR51,AS51,AT51,AU51,AV51,AW51,AX51,AY51,AZ51,BA51,BB51,BC51,BD51,BE51,BF51,BG51,BH51,BI51,BJ51,BK51,BL51)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH48</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B51,AI51,AJ51,AK51,AL51,AM51,AN51,AO51,AP51,AQ51,AR51,AS51,AT51,AU51,AV51,AW51,AX51,AY51,AZ51,BA51,BB51,BC51,BD51,BE51,BF51,BG51,BH51,BI51,BJ51,BK51,BL51)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH48</v>
       </c>
       <c r="AI51" s="0" t="str">
         <f aca="false">IF(D51="y", " --"&amp;D$1,IF(NOT(ISBLANK(D51))," --"&amp;D$1&amp;" "&amp;D51,""))</f>
@@ -21433,13 +21508,14 @@
         <v/>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="n">
         <v>49</v>
       </c>
+      <c r="F52" s="2"/>
       <c r="AH52" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B52,AI52,AJ52,AK52,AL52,AM52,AN52,AO52,AP52,AQ52,AR52,AS52,AT52,AU52,AV52,AW52,AX52,AY52,AZ52,BA52,BB52,BC52,BD52,BE52,BF52,BG52,BH52,BI52,BJ52,BK52,BL52)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH49</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B52,AI52,AJ52,AK52,AL52,AM52,AN52,AO52,AP52,AQ52,AR52,AS52,AT52,AU52,AV52,AW52,AX52,AY52,AZ52,BA52,BB52,BC52,BD52,BE52,BF52,BG52,BH52,BI52,BJ52,BK52,BL52)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH49</v>
       </c>
       <c r="AI52" s="0" t="str">
         <f aca="false">IF(D52="y", " --"&amp;D$1,IF(NOT(ISBLANK(D52))," --"&amp;D$1&amp;" "&amp;D52,""))</f>
@@ -21558,13 +21634,14 @@
         <v/>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="F53" s="2"/>
       <c r="AH53" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B53,AI53,AJ53,AK53,AL53,AM53,AN53,AO53,AP53,AQ53,AR53,AS53,AT53,AU53,AV53,AW53,AX53,AY53,AZ53,BA53,BB53,BC53,BD53,BE53,BF53,BG53,BH53,BI53,BJ53,BK53,BL53)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH50</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B53,AI53,AJ53,AK53,AL53,AM53,AN53,AO53,AP53,AQ53,AR53,AS53,AT53,AU53,AV53,AW53,AX53,AY53,AZ53,BA53,BB53,BC53,BD53,BE53,BF53,BG53,BH53,BI53,BJ53,BK53,BL53)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH50</v>
       </c>
       <c r="AI53" s="0" t="str">
         <f aca="false">IF(D53="y", " --"&amp;D$1,IF(NOT(ISBLANK(D53))," --"&amp;D$1&amp;" "&amp;D53,""))</f>
@@ -21683,13 +21760,14 @@
         <v/>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="n">
         <v>51</v>
       </c>
+      <c r="F54" s="2"/>
       <c r="AH54" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B54,AI54,AJ54,AK54,AL54,AM54,AN54,AO54,AP54,AQ54,AR54,AS54,AT54,AU54,AV54,AW54,AX54,AY54,AZ54,BA54,BB54,BC54,BD54,BE54,BF54,BG54,BH54,BI54,BJ54,BK54,BL54)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH51</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B54,AI54,AJ54,AK54,AL54,AM54,AN54,AO54,AP54,AQ54,AR54,AS54,AT54,AU54,AV54,AW54,AX54,AY54,AZ54,BA54,BB54,BC54,BD54,BE54,BF54,BG54,BH54,BI54,BJ54,BK54,BL54)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH51</v>
       </c>
       <c r="AI54" s="0" t="str">
         <f aca="false">IF(D54="y", " --"&amp;D$1,IF(NOT(ISBLANK(D54))," --"&amp;D$1&amp;" "&amp;D54,""))</f>
@@ -21808,13 +21886,14 @@
         <v/>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="n">
         <v>52</v>
       </c>
+      <c r="F55" s="2"/>
       <c r="AH55" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B55,AI55,AJ55,AK55,AL55,AM55,AN55,AO55,AP55,AQ55,AR55,AS55,AT55,AU55,AV55,AW55,AX55,AY55,AZ55,BA55,BB55,BC55,BD55,BE55,BF55,BG55,BH55,BI55,BJ55,BK55,BL55)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH52</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B55,AI55,AJ55,AK55,AL55,AM55,AN55,AO55,AP55,AQ55,AR55,AS55,AT55,AU55,AV55,AW55,AX55,AY55,AZ55,BA55,BB55,BC55,BD55,BE55,BF55,BG55,BH55,BI55,BJ55,BK55,BL55)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH52</v>
       </c>
       <c r="AI55" s="0" t="str">
         <f aca="false">IF(D55="y", " --"&amp;D$1,IF(NOT(ISBLANK(D55))," --"&amp;D$1&amp;" "&amp;D55,""))</f>
@@ -21933,13 +22012,13 @@
         <v/>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="n">
         <v>53</v>
       </c>
       <c r="AH56" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B56,AI56,AJ56,AK56,AL56,AM56,AN56,AO56,AP56,AQ56,AR56,AS56,AT56,AU56,AV56,AW56,AX56,AY56,AZ56,BA56,BB56,BC56,BD56,BE56,BF56,BG56,BH56,BI56,BJ56,BK56,BL56)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH53</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B56,AI56,AJ56,AK56,AL56,AM56,AN56,AO56,AP56,AQ56,AR56,AS56,AT56,AU56,AV56,AW56,AX56,AY56,AZ56,BA56,BB56,BC56,BD56,BE56,BF56,BG56,BH56,BI56,BJ56,BK56,BL56)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH53</v>
       </c>
       <c r="AI56" s="0" t="str">
         <f aca="false">IF(D56="y", " --"&amp;D$1,IF(NOT(ISBLANK(D56))," --"&amp;D$1&amp;" "&amp;D56,""))</f>
@@ -22058,13 +22137,13 @@
         <v/>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="n">
         <v>54</v>
       </c>
       <c r="AH57" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B57,AI57,AJ57,AK57,AL57,AM57,AN57,AO57,AP57,AQ57,AR57,AS57,AT57,AU57,AV57,AW57,AX57,AY57,AZ57,BA57,BB57,BC57,BD57,BE57,BF57,BG57,BH57,BI57,BJ57,BK57,BL57)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH54</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B57,AI57,AJ57,AK57,AL57,AM57,AN57,AO57,AP57,AQ57,AR57,AS57,AT57,AU57,AV57,AW57,AX57,AY57,AZ57,BA57,BB57,BC57,BD57,BE57,BF57,BG57,BH57,BI57,BJ57,BK57,BL57)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH54</v>
       </c>
       <c r="AI57" s="0" t="str">
         <f aca="false">IF(D57="y", " --"&amp;D$1,IF(NOT(ISBLANK(D57))," --"&amp;D$1&amp;" "&amp;D57,""))</f>
@@ -22183,13 +22262,13 @@
         <v/>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="n">
         <v>55</v>
       </c>
       <c r="AH58" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B58,AI58,AJ58,AK58,AL58,AM58,AN58,AO58,AP58,AQ58,AR58,AS58,AT58,AU58,AV58,AW58,AX58,AY58,AZ58,BA58,BB58,BC58,BD58,BE58,BF58,BG58,BH58,BI58,BJ58,BK58,BL58)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH55</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B58,AI58,AJ58,AK58,AL58,AM58,AN58,AO58,AP58,AQ58,AR58,AS58,AT58,AU58,AV58,AW58,AX58,AY58,AZ58,BA58,BB58,BC58,BD58,BE58,BF58,BG58,BH58,BI58,BJ58,BK58,BL58)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH55</v>
       </c>
       <c r="AI58" s="0" t="str">
         <f aca="false">IF(D58="y", " --"&amp;D$1,IF(NOT(ISBLANK(D58))," --"&amp;D$1&amp;" "&amp;D58,""))</f>
@@ -22308,13 +22387,13 @@
         <v/>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="n">
         <v>56</v>
       </c>
       <c r="AH59" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B59,AI59,AJ59,AK59,AL59,AM59,AN59,AO59,AP59,AQ59,AR59,AS59,AT59,AU59,AV59,AW59,AX59,AY59,AZ59,BA59,BB59,BC59,BD59,BE59,BF59,BG59,BH59,BI59,BJ59,BK59,BL59)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH56</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B59,AI59,AJ59,AK59,AL59,AM59,AN59,AO59,AP59,AQ59,AR59,AS59,AT59,AU59,AV59,AW59,AX59,AY59,AZ59,BA59,BB59,BC59,BD59,BE59,BF59,BG59,BH59,BI59,BJ59,BK59,BL59)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH56</v>
       </c>
       <c r="AI59" s="0" t="str">
         <f aca="false">IF(D59="y", " --"&amp;D$1,IF(NOT(ISBLANK(D59))," --"&amp;D$1&amp;" "&amp;D59,""))</f>
@@ -22433,13 +22512,13 @@
         <v/>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="n">
         <v>57</v>
       </c>
       <c r="AH60" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B60,AI60,AJ60,AK60,AL60,AM60,AN60,AO60,AP60,AQ60,AR60,AS60,AT60,AU60,AV60,AW60,AX60,AY60,AZ60,BA60,BB60,BC60,BD60,BE60,BF60,BG60,BH60,BI60,BJ60,BK60,BL60)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH57</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B60,AI60,AJ60,AK60,AL60,AM60,AN60,AO60,AP60,AQ60,AR60,AS60,AT60,AU60,AV60,AW60,AX60,AY60,AZ60,BA60,BB60,BC60,BD60,BE60,BF60,BG60,BH60,BI60,BJ60,BK60,BL60)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH57</v>
       </c>
       <c r="AI60" s="0" t="str">
         <f aca="false">IF(D60="y", " --"&amp;D$1,IF(NOT(ISBLANK(D60))," --"&amp;D$1&amp;" "&amp;D60,""))</f>
@@ -22558,13 +22637,13 @@
         <v/>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="n">
         <v>58</v>
       </c>
       <c r="AH61" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B61,AI61,AJ61,AK61,AL61,AM61,AN61,AO61,AP61,AQ61,AR61,AS61,AT61,AU61,AV61,AW61,AX61,AY61,AZ61,BA61,BB61,BC61,BD61,BE61,BF61,BG61,BH61,BI61,BJ61,BK61,BL61)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH58</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B61,AI61,AJ61,AK61,AL61,AM61,AN61,AO61,AP61,AQ61,AR61,AS61,AT61,AU61,AV61,AW61,AX61,AY61,AZ61,BA61,BB61,BC61,BD61,BE61,BF61,BG61,BH61,BI61,BJ61,BK61,BL61)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH58</v>
       </c>
       <c r="AI61" s="0" t="str">
         <f aca="false">IF(D61="y", " --"&amp;D$1,IF(NOT(ISBLANK(D61))," --"&amp;D$1&amp;" "&amp;D61,""))</f>
@@ -22683,13 +22762,13 @@
         <v/>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="n">
         <v>59</v>
       </c>
       <c r="AH62" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B62,AI62,AJ62,AK62,AL62,AM62,AN62,AO62,AP62,AQ62,AR62,AS62,AT62,AU62,AV62,AW62,AX62,AY62,AZ62,BA62,BB62,BC62,BD62,BE62,BF62,BG62,BH62,BI62,BJ62,BK62,BL62)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH59</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B62,AI62,AJ62,AK62,AL62,AM62,AN62,AO62,AP62,AQ62,AR62,AS62,AT62,AU62,AV62,AW62,AX62,AY62,AZ62,BA62,BB62,BC62,BD62,BE62,BF62,BG62,BH62,BI62,BJ62,BK62,BL62)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH59</v>
       </c>
       <c r="AI62" s="0" t="str">
         <f aca="false">IF(D62="y", " --"&amp;D$1,IF(NOT(ISBLANK(D62))," --"&amp;D$1&amp;" "&amp;D62,""))</f>
@@ -22808,13 +22887,13 @@
         <v/>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="n">
         <v>60</v>
       </c>
       <c r="AH63" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B63,AI63,AJ63,AK63,AL63,AM63,AN63,AO63,AP63,AQ63,AR63,AS63,AT63,AU63,AV63,AW63,AX63,AY63,AZ63,BA63,BB63,BC63,BD63,BE63,BF63,BG63,BH63,BI63,BJ63,BK63,BL63)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH60</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B63,AI63,AJ63,AK63,AL63,AM63,AN63,AO63,AP63,AQ63,AR63,AS63,AT63,AU63,AV63,AW63,AX63,AY63,AZ63,BA63,BB63,BC63,BD63,BE63,BF63,BG63,BH63,BI63,BJ63,BK63,BL63)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH60</v>
       </c>
       <c r="AI63" s="0" t="str">
         <f aca="false">IF(D63="y", " --"&amp;D$1,IF(NOT(ISBLANK(D63))," --"&amp;D$1&amp;" "&amp;D63,""))</f>
@@ -22933,13 +23012,13 @@
         <v/>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="n">
         <v>61</v>
       </c>
       <c r="AH64" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B64,AI64,AJ64,AK64,AL64,AM64,AN64,AO64,AP64,AQ64,AR64,AS64,AT64,AU64,AV64,AW64,AX64,AY64,AZ64,BA64,BB64,BC64,BD64,BE64,BF64,BG64,BH64,BI64,BJ64,BK64,BL64)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH61</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B64,AI64,AJ64,AK64,AL64,AM64,AN64,AO64,AP64,AQ64,AR64,AS64,AT64,AU64,AV64,AW64,AX64,AY64,AZ64,BA64,BB64,BC64,BD64,BE64,BF64,BG64,BH64,BI64,BJ64,BK64,BL64)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH61</v>
       </c>
       <c r="AI64" s="0" t="str">
         <f aca="false">IF(D64="y", " --"&amp;D$1,IF(NOT(ISBLANK(D64))," --"&amp;D$1&amp;" "&amp;D64,""))</f>
@@ -23058,13 +23137,13 @@
         <v/>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="n">
         <v>62</v>
       </c>
       <c r="AH65" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B65,AI65,AJ65,AK65,AL65,AM65,AN65,AO65,AP65,AQ65,AR65,AS65,AT65,AU65,AV65,AW65,AX65,AY65,AZ65,BA65,BB65,BC65,BD65,BE65,BF65,BG65,BH65,BI65,BJ65,BK65,BL65)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH62</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B65,AI65,AJ65,AK65,AL65,AM65,AN65,AO65,AP65,AQ65,AR65,AS65,AT65,AU65,AV65,AW65,AX65,AY65,AZ65,BA65,BB65,BC65,BD65,BE65,BF65,BG65,BH65,BI65,BJ65,BK65,BL65)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH62</v>
       </c>
       <c r="AI65" s="0" t="str">
         <f aca="false">IF(D65="y", " --"&amp;D$1,IF(NOT(ISBLANK(D65))," --"&amp;D$1&amp;" "&amp;D65,""))</f>
@@ -23183,13 +23262,13 @@
         <v/>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="n">
         <v>63</v>
       </c>
       <c r="AH66" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B66,AI66,AJ66,AK66,AL66,AM66,AN66,AO66,AP66,AQ66,AR66,AS66,AT66,AU66,AV66,AW66,AX66,AY66,AZ66,BA66,BB66,BC66,BD66,BE66,BF66,BG66,BH66,BI66,BJ66,BK66,BL66)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH63</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B66,AI66,AJ66,AK66,AL66,AM66,AN66,AO66,AP66,AQ66,AR66,AS66,AT66,AU66,AV66,AW66,AX66,AY66,AZ66,BA66,BB66,BC66,BD66,BE66,BF66,BG66,BH66,BI66,BJ66,BK66,BL66)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH63</v>
       </c>
       <c r="AI66" s="0" t="str">
         <f aca="false">IF(D66="y", " --"&amp;D$1,IF(NOT(ISBLANK(D66))," --"&amp;D$1&amp;" "&amp;D66,""))</f>
@@ -23308,13 +23387,13 @@
         <v/>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="n">
         <v>64</v>
       </c>
       <c r="AH67" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B67,AI67,AJ67,AK67,AL67,AM67,AN67,AO67,AP67,AQ67,AR67,AS67,AT67,AU67,AV67,AW67,AX67,AY67,AZ67,BA67,BB67,BC67,BD67,BE67,BF67,BG67,BH67,BI67,BJ67,BK67,BL67)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH64</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B67,AI67,AJ67,AK67,AL67,AM67,AN67,AO67,AP67,AQ67,AR67,AS67,AT67,AU67,AV67,AW67,AX67,AY67,AZ67,BA67,BB67,BC67,BD67,BE67,BF67,BG67,BH67,BI67,BJ67,BK67,BL67)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH64</v>
       </c>
       <c r="AI67" s="0" t="str">
         <f aca="false">IF(D67="y", " --"&amp;D$1,IF(NOT(ISBLANK(D67))," --"&amp;D$1&amp;" "&amp;D67,""))</f>
@@ -23433,13 +23512,13 @@
         <v/>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="n">
         <v>65</v>
       </c>
       <c r="AH68" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B68,AI68,AJ68,AK68,AL68,AM68,AN68,AO68,AP68,AQ68,AR68,AS68,AT68,AU68,AV68,AW68,AX68,AY68,AZ68,BA68,BB68,BC68,BD68,BE68,BF68,BG68,BH68,BI68,BJ68,BK68,BL68)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH65</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B68,AI68,AJ68,AK68,AL68,AM68,AN68,AO68,AP68,AQ68,AR68,AS68,AT68,AU68,AV68,AW68,AX68,AY68,AZ68,BA68,BB68,BC68,BD68,BE68,BF68,BG68,BH68,BI68,BJ68,BK68,BL68)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH65</v>
       </c>
       <c r="AI68" s="0" t="str">
         <f aca="false">IF(D68="y", " --"&amp;D$1,IF(NOT(ISBLANK(D68))," --"&amp;D$1&amp;" "&amp;D68,""))</f>
@@ -23558,13 +23637,13 @@
         <v/>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="n">
         <v>66</v>
       </c>
       <c r="AH69" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B69,AI69,AJ69,AK69,AL69,AM69,AN69,AO69,AP69,AQ69,AR69,AS69,AT69,AU69,AV69,AW69,AX69,AY69,AZ69,BA69,BB69,BC69,BD69,BE69,BF69,BG69,BH69,BI69,BJ69,BK69,BL69)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH66</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B69,AI69,AJ69,AK69,AL69,AM69,AN69,AO69,AP69,AQ69,AR69,AS69,AT69,AU69,AV69,AW69,AX69,AY69,AZ69,BA69,BB69,BC69,BD69,BE69,BF69,BG69,BH69,BI69,BJ69,BK69,BL69)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH66</v>
       </c>
       <c r="AI69" s="0" t="str">
         <f aca="false">IF(D69="y", " --"&amp;D$1,IF(NOT(ISBLANK(D69))," --"&amp;D$1&amp;" "&amp;D69,""))</f>
@@ -23683,13 +23762,13 @@
         <v/>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="n">
         <v>67</v>
       </c>
       <c r="AH70" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B70,AI70,AJ70,AK70,AL70,AM70,AN70,AO70,AP70,AQ70,AR70,AS70,AT70,AU70,AV70,AW70,AX70,AY70,AZ70,BA70,BB70,BC70,BD70,BE70,BF70,BG70,BH70,BI70,BJ70,BK70,BL70)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH67</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B70,AI70,AJ70,AK70,AL70,AM70,AN70,AO70,AP70,AQ70,AR70,AS70,AT70,AU70,AV70,AW70,AX70,AY70,AZ70,BA70,BB70,BC70,BD70,BE70,BF70,BG70,BH70,BI70,BJ70,BK70,BL70)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH67</v>
       </c>
       <c r="AI70" s="0" t="str">
         <f aca="false">IF(D70="y", " --"&amp;D$1,IF(NOT(ISBLANK(D70))," --"&amp;D$1&amp;" "&amp;D70,""))</f>
@@ -23808,13 +23887,13 @@
         <v/>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="n">
         <v>68</v>
       </c>
       <c r="AH71" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B71,AI71,AJ71,AK71,AL71,AM71,AN71,AO71,AP71,AQ71,AR71,AS71,AT71,AU71,AV71,AW71,AX71,AY71,AZ71,BA71,BB71,BC71,BD71,BE71,BF71,BG71,BH71,BI71,BJ71,BK71,BL71)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH68</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B71,AI71,AJ71,AK71,AL71,AM71,AN71,AO71,AP71,AQ71,AR71,AS71,AT71,AU71,AV71,AW71,AX71,AY71,AZ71,BA71,BB71,BC71,BD71,BE71,BF71,BG71,BH71,BI71,BJ71,BK71,BL71)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH68</v>
       </c>
       <c r="AI71" s="0" t="str">
         <f aca="false">IF(D71="y", " --"&amp;D$1,IF(NOT(ISBLANK(D71))," --"&amp;D$1&amp;" "&amp;D71,""))</f>
@@ -23933,13 +24012,13 @@
         <v/>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="n">
         <v>69</v>
       </c>
       <c r="AH72" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B72,AI72,AJ72,AK72,AL72,AM72,AN72,AO72,AP72,AQ72,AR72,AS72,AT72,AU72,AV72,AW72,AX72,AY72,AZ72,BA72,BB72,BC72,BD72,BE72,BF72,BG72,BH72,BI72,BJ72,BK72,BL72)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH69</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B72,AI72,AJ72,AK72,AL72,AM72,AN72,AO72,AP72,AQ72,AR72,AS72,AT72,AU72,AV72,AW72,AX72,AY72,AZ72,BA72,BB72,BC72,BD72,BE72,BF72,BG72,BH72,BI72,BJ72,BK72,BL72)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH69</v>
       </c>
       <c r="AI72" s="0" t="str">
         <f aca="false">IF(D72="y", " --"&amp;D$1,IF(NOT(ISBLANK(D72))," --"&amp;D$1&amp;" "&amp;D72,""))</f>
@@ -24058,13 +24137,13 @@
         <v/>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="n">
         <v>70</v>
       </c>
       <c r="AH73" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B73,AI73,AJ73,AK73,AL73,AM73,AN73,AO73,AP73,AQ73,AR73,AS73,AT73,AU73,AV73,AW73,AX73,AY73,AZ73,BA73,BB73,BC73,BD73,BE73,BF73,BG73,BH73,BI73,BJ73,BK73,BL73)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH70</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B73,AI73,AJ73,AK73,AL73,AM73,AN73,AO73,AP73,AQ73,AR73,AS73,AT73,AU73,AV73,AW73,AX73,AY73,AZ73,BA73,BB73,BC73,BD73,BE73,BF73,BG73,BH73,BI73,BJ73,BK73,BL73)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH70</v>
       </c>
       <c r="AI73" s="0" t="str">
         <f aca="false">IF(D73="y", " --"&amp;D$1,IF(NOT(ISBLANK(D73))," --"&amp;D$1&amp;" "&amp;D73,""))</f>
@@ -24183,13 +24262,13 @@
         <v/>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="n">
         <v>71</v>
       </c>
       <c r="AH74" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B74,AI74,AJ74,AK74,AL74,AM74,AN74,AO74,AP74,AQ74,AR74,AS74,AT74,AU74,AV74,AW74,AX74,AY74,AZ74,BA74,BB74,BC74,BD74,BE74,BF74,BG74,BH74,BI74,BJ74,BK74,BL74)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH71</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B74,AI74,AJ74,AK74,AL74,AM74,AN74,AO74,AP74,AQ74,AR74,AS74,AT74,AU74,AV74,AW74,AX74,AY74,AZ74,BA74,BB74,BC74,BD74,BE74,BF74,BG74,BH74,BI74,BJ74,BK74,BL74)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH71</v>
       </c>
       <c r="AI74" s="0" t="str">
         <f aca="false">IF(D74="y", " --"&amp;D$1,IF(NOT(ISBLANK(D74))," --"&amp;D$1&amp;" "&amp;D74,""))</f>
@@ -24308,13 +24387,13 @@
         <v/>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="n">
         <v>72</v>
       </c>
       <c r="AH75" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B75,AI75,AJ75,AK75,AL75,AM75,AN75,AO75,AP75,AQ75,AR75,AS75,AT75,AU75,AV75,AW75,AX75,AY75,AZ75,BA75,BB75,BC75,BD75,BE75,BF75,BG75,BH75,BI75,BJ75,BK75,BL75)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH72</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B75,AI75,AJ75,AK75,AL75,AM75,AN75,AO75,AP75,AQ75,AR75,AS75,AT75,AU75,AV75,AW75,AX75,AY75,AZ75,BA75,BB75,BC75,BD75,BE75,BF75,BG75,BH75,BI75,BJ75,BK75,BL75)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH72</v>
       </c>
       <c r="AI75" s="0" t="str">
         <f aca="false">IF(D75="y", " --"&amp;D$1,IF(NOT(ISBLANK(D75))," --"&amp;D$1&amp;" "&amp;D75,""))</f>
@@ -24433,13 +24512,13 @@
         <v/>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="n">
         <v>73</v>
       </c>
       <c r="AH76" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B76,AI76,AJ76,AK76,AL76,AM76,AN76,AO76,AP76,AQ76,AR76,AS76,AT76,AU76,AV76,AW76,AX76,AY76,AZ76,BA76,BB76,BC76,BD76,BE76,BF76,BG76,BH76,BI76,BJ76,BK76,BL76)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH73</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B76,AI76,AJ76,AK76,AL76,AM76,AN76,AO76,AP76,AQ76,AR76,AS76,AT76,AU76,AV76,AW76,AX76,AY76,AZ76,BA76,BB76,BC76,BD76,BE76,BF76,BG76,BH76,BI76,BJ76,BK76,BL76)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH73</v>
       </c>
       <c r="AI76" s="0" t="str">
         <f aca="false">IF(D76="y", " --"&amp;D$1,IF(NOT(ISBLANK(D76))," --"&amp;D$1&amp;" "&amp;D76,""))</f>
@@ -24558,13 +24637,13 @@
         <v/>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="n">
         <v>74</v>
       </c>
       <c r="AH77" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B77,AI77,AJ77,AK77,AL77,AM77,AN77,AO77,AP77,AQ77,AR77,AS77,AT77,AU77,AV77,AW77,AX77,AY77,AZ77,BA77,BB77,BC77,BD77,BE77,BF77,BG77,BH77,BI77,BJ77,BK77,BL77)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH74</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B77,AI77,AJ77,AK77,AL77,AM77,AN77,AO77,AP77,AQ77,AR77,AS77,AT77,AU77,AV77,AW77,AX77,AY77,AZ77,BA77,BB77,BC77,BD77,BE77,BF77,BG77,BH77,BI77,BJ77,BK77,BL77)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH74</v>
       </c>
       <c r="AI77" s="0" t="str">
         <f aca="false">IF(D77="y", " --"&amp;D$1,IF(NOT(ISBLANK(D77))," --"&amp;D$1&amp;" "&amp;D77,""))</f>
@@ -24683,13 +24762,13 @@
         <v/>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="n">
         <v>75</v>
       </c>
       <c r="AH78" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B78,AI78,AJ78,AK78,AL78,AM78,AN78,AO78,AP78,AQ78,AR78,AS78,AT78,AU78,AV78,AW78,AX78,AY78,AZ78,BA78,BB78,BC78,BD78,BE78,BF78,BG78,BH78,BI78,BJ78,BK78,BL78)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH75</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B78,AI78,AJ78,AK78,AL78,AM78,AN78,AO78,AP78,AQ78,AR78,AS78,AT78,AU78,AV78,AW78,AX78,AY78,AZ78,BA78,BB78,BC78,BD78,BE78,BF78,BG78,BH78,BI78,BJ78,BK78,BL78)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH75</v>
       </c>
       <c r="AI78" s="0" t="str">
         <f aca="false">IF(D78="y", " --"&amp;D$1,IF(NOT(ISBLANK(D78))," --"&amp;D$1&amp;" "&amp;D78,""))</f>
@@ -24808,13 +24887,13 @@
         <v/>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="n">
         <v>76</v>
       </c>
       <c r="AH79" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B79,AI79,AJ79,AK79,AL79,AM79,AN79,AO79,AP79,AQ79,AR79,AS79,AT79,AU79,AV79,AW79,AX79,AY79,AZ79,BA79,BB79,BC79,BD79,BE79,BF79,BG79,BH79,BI79,BJ79,BK79,BL79)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH76</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B79,AI79,AJ79,AK79,AL79,AM79,AN79,AO79,AP79,AQ79,AR79,AS79,AT79,AU79,AV79,AW79,AX79,AY79,AZ79,BA79,BB79,BC79,BD79,BE79,BF79,BG79,BH79,BI79,BJ79,BK79,BL79)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH76</v>
       </c>
       <c r="AI79" s="0" t="str">
         <f aca="false">IF(D79="y", " --"&amp;D$1,IF(NOT(ISBLANK(D79))," --"&amp;D$1&amp;" "&amp;D79,""))</f>
@@ -24933,13 +25012,13 @@
         <v/>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="n">
         <v>77</v>
       </c>
       <c r="AH80" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B80,AI80,AJ80,AK80,AL80,AM80,AN80,AO80,AP80,AQ80,AR80,AS80,AT80,AU80,AV80,AW80,AX80,AY80,AZ80,BA80,BB80,BC80,BD80,BE80,BF80,BG80,BH80,BI80,BJ80,BK80,BL80)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH77</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B80,AI80,AJ80,AK80,AL80,AM80,AN80,AO80,AP80,AQ80,AR80,AS80,AT80,AU80,AV80,AW80,AX80,AY80,AZ80,BA80,BB80,BC80,BD80,BE80,BF80,BG80,BH80,BI80,BJ80,BK80,BL80)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH77</v>
       </c>
       <c r="AI80" s="0" t="str">
         <f aca="false">IF(D80="y", " --"&amp;D$1,IF(NOT(ISBLANK(D80))," --"&amp;D$1&amp;" "&amp;D80,""))</f>
@@ -25058,13 +25137,13 @@
         <v/>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="n">
         <v>78</v>
       </c>
       <c r="AH81" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B81,AI81,AJ81,AK81,AL81,AM81,AN81,AO81,AP81,AQ81,AR81,AS81,AT81,AU81,AV81,AW81,AX81,AY81,AZ81,BA81,BB81,BC81,BD81,BE81,BF81,BG81,BH81,BI81,BJ81,BK81,BL81)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH78</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B81,AI81,AJ81,AK81,AL81,AM81,AN81,AO81,AP81,AQ81,AR81,AS81,AT81,AU81,AV81,AW81,AX81,AY81,AZ81,BA81,BB81,BC81,BD81,BE81,BF81,BG81,BH81,BI81,BJ81,BK81,BL81)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH78</v>
       </c>
       <c r="AI81" s="0" t="str">
         <f aca="false">IF(D81="y", " --"&amp;D$1,IF(NOT(ISBLANK(D81))," --"&amp;D$1&amp;" "&amp;D81,""))</f>
@@ -25183,13 +25262,13 @@
         <v/>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="n">
         <v>79</v>
       </c>
       <c r="AH82" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B82,AI82,AJ82,AK82,AL82,AM82,AN82,AO82,AP82,AQ82,AR82,AS82,AT82,AU82,AV82,AW82,AX82,AY82,AZ82,BA82,BB82,BC82,BD82,BE82,BF82,BG82,BH82,BI82,BJ82,BK82,BL82)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH79</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B82,AI82,AJ82,AK82,AL82,AM82,AN82,AO82,AP82,AQ82,AR82,AS82,AT82,AU82,AV82,AW82,AX82,AY82,AZ82,BA82,BB82,BC82,BD82,BE82,BF82,BG82,BH82,BI82,BJ82,BK82,BL82)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH79</v>
       </c>
       <c r="AI82" s="0" t="str">
         <f aca="false">IF(D82="y", " --"&amp;D$1,IF(NOT(ISBLANK(D82))," --"&amp;D$1&amp;" "&amp;D82,""))</f>
@@ -25308,13 +25387,13 @@
         <v/>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="n">
         <v>80</v>
       </c>
       <c r="AH83" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B83,AI83,AJ83,AK83,AL83,AM83,AN83,AO83,AP83,AQ83,AR83,AS83,AT83,AU83,AV83,AW83,AX83,AY83,AZ83,BA83,BB83,BC83,BD83,BE83,BF83,BG83,BH83,BI83,BJ83,BK83,BL83)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH80</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B83,AI83,AJ83,AK83,AL83,AM83,AN83,AO83,AP83,AQ83,AR83,AS83,AT83,AU83,AV83,AW83,AX83,AY83,AZ83,BA83,BB83,BC83,BD83,BE83,BF83,BG83,BH83,BI83,BJ83,BK83,BL83)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH80</v>
       </c>
       <c r="AI83" s="0" t="str">
         <f aca="false">IF(D83="y", " --"&amp;D$1,IF(NOT(ISBLANK(D83))," --"&amp;D$1&amp;" "&amp;D83,""))</f>
@@ -25433,13 +25512,13 @@
         <v/>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="n">
         <v>81</v>
       </c>
       <c r="AH84" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B84,AI84,AJ84,AK84,AL84,AM84,AN84,AO84,AP84,AQ84,AR84,AS84,AT84,AU84,AV84,AW84,AX84,AY84,AZ84,BA84,BB84,BC84,BD84,BE84,BF84,BG84,BH84,BI84,BJ84,BK84,BL84)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH81</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B84,AI84,AJ84,AK84,AL84,AM84,AN84,AO84,AP84,AQ84,AR84,AS84,AT84,AU84,AV84,AW84,AX84,AY84,AZ84,BA84,BB84,BC84,BD84,BE84,BF84,BG84,BH84,BI84,BJ84,BK84,BL84)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH81</v>
       </c>
       <c r="AI84" s="0" t="str">
         <f aca="false">IF(D84="y", " --"&amp;D$1,IF(NOT(ISBLANK(D84))," --"&amp;D$1&amp;" "&amp;D84,""))</f>
@@ -25558,13 +25637,13 @@
         <v/>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="n">
         <v>82</v>
       </c>
       <c r="AH85" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B85,AI85,AJ85,AK85,AL85,AM85,AN85,AO85,AP85,AQ85,AR85,AS85,AT85,AU85,AV85,AW85,AX85,AY85,AZ85,BA85,BB85,BC85,BD85,BE85,BF85,BG85,BH85,BI85,BJ85,BK85,BL85)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH82</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B85,AI85,AJ85,AK85,AL85,AM85,AN85,AO85,AP85,AQ85,AR85,AS85,AT85,AU85,AV85,AW85,AX85,AY85,AZ85,BA85,BB85,BC85,BD85,BE85,BF85,BG85,BH85,BI85,BJ85,BK85,BL85)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH82</v>
       </c>
       <c r="AI85" s="0" t="str">
         <f aca="false">IF(D85="y", " --"&amp;D$1,IF(NOT(ISBLANK(D85))," --"&amp;D$1&amp;" "&amp;D85,""))</f>
@@ -25683,13 +25762,13 @@
         <v/>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="n">
         <v>83</v>
       </c>
       <c r="AH86" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B86,AI86,AJ86,AK86,AL86,AM86,AN86,AO86,AP86,AQ86,AR86,AS86,AT86,AU86,AV86,AW86,AX86,AY86,AZ86,BA86,BB86,BC86,BD86,BE86,BF86,BG86,BH86,BI86,BJ86,BK86,BL86)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH83</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B86,AI86,AJ86,AK86,AL86,AM86,AN86,AO86,AP86,AQ86,AR86,AS86,AT86,AU86,AV86,AW86,AX86,AY86,AZ86,BA86,BB86,BC86,BD86,BE86,BF86,BG86,BH86,BI86,BJ86,BK86,BL86)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH83</v>
       </c>
       <c r="AI86" s="0" t="str">
         <f aca="false">IF(D86="y", " --"&amp;D$1,IF(NOT(ISBLANK(D86))," --"&amp;D$1&amp;" "&amp;D86,""))</f>
@@ -25808,13 +25887,13 @@
         <v/>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="n">
         <v>84</v>
       </c>
       <c r="AH87" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B87,AI87,AJ87,AK87,AL87,AM87,AN87,AO87,AP87,AQ87,AR87,AS87,AT87,AU87,AV87,AW87,AX87,AY87,AZ87,BA87,BB87,BC87,BD87,BE87,BF87,BG87,BH87,BI87,BJ87,BK87,BL87)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH84</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B87,AI87,AJ87,AK87,AL87,AM87,AN87,AO87,AP87,AQ87,AR87,AS87,AT87,AU87,AV87,AW87,AX87,AY87,AZ87,BA87,BB87,BC87,BD87,BE87,BF87,BG87,BH87,BI87,BJ87,BK87,BL87)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH84</v>
       </c>
       <c r="AI87" s="0" t="str">
         <f aca="false">IF(D87="y", " --"&amp;D$1,IF(NOT(ISBLANK(D87))," --"&amp;D$1&amp;" "&amp;D87,""))</f>
@@ -25933,13 +26012,13 @@
         <v/>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="n">
         <v>85</v>
       </c>
       <c r="AH88" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B88,AI88,AJ88,AK88,AL88,AM88,AN88,AO88,AP88,AQ88,AR88,AS88,AT88,AU88,AV88,AW88,AX88,AY88,AZ88,BA88,BB88,BC88,BD88,BE88,BF88,BG88,BH88,BI88,BJ88,BK88,BL88)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH85</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B88,AI88,AJ88,AK88,AL88,AM88,AN88,AO88,AP88,AQ88,AR88,AS88,AT88,AU88,AV88,AW88,AX88,AY88,AZ88,BA88,BB88,BC88,BD88,BE88,BF88,BG88,BH88,BI88,BJ88,BK88,BL88)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH85</v>
       </c>
       <c r="AI88" s="0" t="str">
         <f aca="false">IF(D88="y", " --"&amp;D$1,IF(NOT(ISBLANK(D88))," --"&amp;D$1&amp;" "&amp;D88,""))</f>
@@ -26058,13 +26137,13 @@
         <v/>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="n">
         <v>86</v>
       </c>
       <c r="AH89" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B89,AI89,AJ89,AK89,AL89,AM89,AN89,AO89,AP89,AQ89,AR89,AS89,AT89,AU89,AV89,AW89,AX89,AY89,AZ89,BA89,BB89,BC89,BD89,BE89,BF89,BG89,BH89,BI89,BJ89,BK89,BL89)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH86</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B89,AI89,AJ89,AK89,AL89,AM89,AN89,AO89,AP89,AQ89,AR89,AS89,AT89,AU89,AV89,AW89,AX89,AY89,AZ89,BA89,BB89,BC89,BD89,BE89,BF89,BG89,BH89,BI89,BJ89,BK89,BL89)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH86</v>
       </c>
       <c r="AI89" s="0" t="str">
         <f aca="false">IF(D89="y", " --"&amp;D$1,IF(NOT(ISBLANK(D89))," --"&amp;D$1&amp;" "&amp;D89,""))</f>
@@ -26183,13 +26262,13 @@
         <v/>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="n">
         <v>87</v>
       </c>
       <c r="AH90" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B90,AI90,AJ90,AK90,AL90,AM90,AN90,AO90,AP90,AQ90,AR90,AS90,AT90,AU90,AV90,AW90,AX90,AY90,AZ90,BA90,BB90,BC90,BD90,BE90,BF90,BG90,BH90,BI90,BJ90,BK90,BL90)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH87</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B90,AI90,AJ90,AK90,AL90,AM90,AN90,AO90,AP90,AQ90,AR90,AS90,AT90,AU90,AV90,AW90,AX90,AY90,AZ90,BA90,BB90,BC90,BD90,BE90,BF90,BG90,BH90,BI90,BJ90,BK90,BL90)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH87</v>
       </c>
       <c r="AI90" s="0" t="str">
         <f aca="false">IF(D90="y", " --"&amp;D$1,IF(NOT(ISBLANK(D90))," --"&amp;D$1&amp;" "&amp;D90,""))</f>
@@ -26308,13 +26387,13 @@
         <v/>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="n">
         <v>88</v>
       </c>
       <c r="AH91" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B91,AI91,AJ91,AK91,AL91,AM91,AN91,AO91,AP91,AQ91,AR91,AS91,AT91,AU91,AV91,AW91,AX91,AY91,AZ91,BA91,BB91,BC91,BD91,BE91,BF91,BG91,BH91,BI91,BJ91,BK91,BL91)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH88</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B91,AI91,AJ91,AK91,AL91,AM91,AN91,AO91,AP91,AQ91,AR91,AS91,AT91,AU91,AV91,AW91,AX91,AY91,AZ91,BA91,BB91,BC91,BD91,BE91,BF91,BG91,BH91,BI91,BJ91,BK91,BL91)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH88</v>
       </c>
       <c r="AI91" s="0" t="str">
         <f aca="false">IF(D91="y", " --"&amp;D$1,IF(NOT(ISBLANK(D91))," --"&amp;D$1&amp;" "&amp;D91,""))</f>
@@ -26433,13 +26512,13 @@
         <v/>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="n">
         <v>89</v>
       </c>
       <c r="AH92" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B92,AI92,AJ92,AK92,AL92,AM92,AN92,AO92,AP92,AQ92,AR92,AS92,AT92,AU92,AV92,AW92,AX92,AY92,AZ92,BA92,BB92,BC92,BD92,BE92,BF92,BG92,BH92,BI92,BJ92,BK92,BL92)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH89</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B92,AI92,AJ92,AK92,AL92,AM92,AN92,AO92,AP92,AQ92,AR92,AS92,AT92,AU92,AV92,AW92,AX92,AY92,AZ92,BA92,BB92,BC92,BD92,BE92,BF92,BG92,BH92,BI92,BJ92,BK92,BL92)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH89</v>
       </c>
       <c r="AI92" s="0" t="str">
         <f aca="false">IF(D92="y", " --"&amp;D$1,IF(NOT(ISBLANK(D92))," --"&amp;D$1&amp;" "&amp;D92,""))</f>
@@ -26558,13 +26637,13 @@
         <v/>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="n">
         <v>90</v>
       </c>
       <c r="AH93" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B93,AI93,AJ93,AK93,AL93,AM93,AN93,AO93,AP93,AQ93,AR93,AS93,AT93,AU93,AV93,AW93,AX93,AY93,AZ93,BA93,BB93,BC93,BD93,BE93,BF93,BG93,BH93,BI93,BJ93,BK93,BL93)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH90</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B93,AI93,AJ93,AK93,AL93,AM93,AN93,AO93,AP93,AQ93,AR93,AS93,AT93,AU93,AV93,AW93,AX93,AY93,AZ93,BA93,BB93,BC93,BD93,BE93,BF93,BG93,BH93,BI93,BJ93,BK93,BL93)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH90</v>
       </c>
       <c r="AI93" s="0" t="str">
         <f aca="false">IF(D93="y", " --"&amp;D$1,IF(NOT(ISBLANK(D93))," --"&amp;D$1&amp;" "&amp;D93,""))</f>
@@ -26683,13 +26762,13 @@
         <v/>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="n">
         <v>91</v>
       </c>
       <c r="AH94" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B94,AI94,AJ94,AK94,AL94,AM94,AN94,AO94,AP94,AQ94,AR94,AS94,AT94,AU94,AV94,AW94,AX94,AY94,AZ94,BA94,BB94,BC94,BD94,BE94,BF94,BG94,BH94,BI94,BJ94,BK94,BL94)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH91</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B94,AI94,AJ94,AK94,AL94,AM94,AN94,AO94,AP94,AQ94,AR94,AS94,AT94,AU94,AV94,AW94,AX94,AY94,AZ94,BA94,BB94,BC94,BD94,BE94,BF94,BG94,BH94,BI94,BJ94,BK94,BL94)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH91</v>
       </c>
       <c r="AI94" s="0" t="str">
         <f aca="false">IF(D94="y", " --"&amp;D$1,IF(NOT(ISBLANK(D94))," --"&amp;D$1&amp;" "&amp;D94,""))</f>
@@ -26808,13 +26887,13 @@
         <v/>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="n">
         <v>92</v>
       </c>
       <c r="AH95" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B95,AI95,AJ95,AK95,AL95,AM95,AN95,AO95,AP95,AQ95,AR95,AS95,AT95,AU95,AV95,AW95,AX95,AY95,AZ95,BA95,BB95,BC95,BD95,BE95,BF95,BG95,BH95,BI95,BJ95,BK95,BL95)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH92</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B95,AI95,AJ95,AK95,AL95,AM95,AN95,AO95,AP95,AQ95,AR95,AS95,AT95,AU95,AV95,AW95,AX95,AY95,AZ95,BA95,BB95,BC95,BD95,BE95,BF95,BG95,BH95,BI95,BJ95,BK95,BL95)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH92</v>
       </c>
       <c r="AI95" s="0" t="str">
         <f aca="false">IF(D95="y", " --"&amp;D$1,IF(NOT(ISBLANK(D95))," --"&amp;D$1&amp;" "&amp;D95,""))</f>
@@ -26933,13 +27012,13 @@
         <v/>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="n">
         <v>93</v>
       </c>
       <c r="AH96" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B96,AI96,AJ96,AK96,AL96,AM96,AN96,AO96,AP96,AQ96,AR96,AS96,AT96,AU96,AV96,AW96,AX96,AY96,AZ96,BA96,BB96,BC96,BD96,BE96,BF96,BG96,BH96,BI96,BJ96,BK96,BL96)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH93</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B96,AI96,AJ96,AK96,AL96,AM96,AN96,AO96,AP96,AQ96,AR96,AS96,AT96,AU96,AV96,AW96,AX96,AY96,AZ96,BA96,BB96,BC96,BD96,BE96,BF96,BG96,BH96,BI96,BJ96,BK96,BL96)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH93</v>
       </c>
       <c r="AI96" s="0" t="str">
         <f aca="false">IF(D96="y", " --"&amp;D$1,IF(NOT(ISBLANK(D96))," --"&amp;D$1&amp;" "&amp;D96,""))</f>
@@ -27058,13 +27137,13 @@
         <v/>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="n">
         <v>94</v>
       </c>
       <c r="AH97" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B97,AI97,AJ97,AK97,AL97,AM97,AN97,AO97,AP97,AQ97,AR97,AS97,AT97,AU97,AV97,AW97,AX97,AY97,AZ97,BA97,BB97,BC97,BD97,BE97,BF97,BG97,BH97,BI97,BJ97,BK97,BL97)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH94</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B97,AI97,AJ97,AK97,AL97,AM97,AN97,AO97,AP97,AQ97,AR97,AS97,AT97,AU97,AV97,AW97,AX97,AY97,AZ97,BA97,BB97,BC97,BD97,BE97,BF97,BG97,BH97,BI97,BJ97,BK97,BL97)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH94</v>
       </c>
       <c r="AI97" s="0" t="str">
         <f aca="false">IF(D97="y", " --"&amp;D$1,IF(NOT(ISBLANK(D97))," --"&amp;D$1&amp;" "&amp;D97,""))</f>
@@ -27183,13 +27262,13 @@
         <v/>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="n">
         <v>95</v>
       </c>
       <c r="AH98" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B98,AI98,AJ98,AK98,AL98,AM98,AN98,AO98,AP98,AQ98,AR98,AS98,AT98,AU98,AV98,AW98,AX98,AY98,AZ98,BA98,BB98,BC98,BD98,BE98,BF98,BG98,BH98,BI98,BJ98,BK98,BL98)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH95</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B98,AI98,AJ98,AK98,AL98,AM98,AN98,AO98,AP98,AQ98,AR98,AS98,AT98,AU98,AV98,AW98,AX98,AY98,AZ98,BA98,BB98,BC98,BD98,BE98,BF98,BG98,BH98,BI98,BJ98,BK98,BL98)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH95</v>
       </c>
       <c r="AI98" s="0" t="str">
         <f aca="false">IF(D98="y", " --"&amp;D$1,IF(NOT(ISBLANK(D98))," --"&amp;D$1&amp;" "&amp;D98,""))</f>
@@ -27308,13 +27387,13 @@
         <v/>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="n">
         <v>96</v>
       </c>
       <c r="AH99" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B99,AI99,AJ99,AK99,AL99,AM99,AN99,AO99,AP99,AQ99,AR99,AS99,AT99,AU99,AV99,AW99,AX99,AY99,AZ99,BA99,BB99,BC99,BD99,BE99,BF99,BG99,BH99,BI99,BJ99,BK99,BL99)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH96</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B99,AI99,AJ99,AK99,AL99,AM99,AN99,AO99,AP99,AQ99,AR99,AS99,AT99,AU99,AV99,AW99,AX99,AY99,AZ99,BA99,BB99,BC99,BD99,BE99,BF99,BG99,BH99,BI99,BJ99,BK99,BL99)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH96</v>
       </c>
       <c r="AI99" s="0" t="str">
         <f aca="false">IF(D99="y", " --"&amp;D$1,IF(NOT(ISBLANK(D99))," --"&amp;D$1&amp;" "&amp;D99,""))</f>
@@ -27433,13 +27512,13 @@
         <v/>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="n">
         <v>97</v>
       </c>
       <c r="AH100" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B100,AI100,AJ100,AK100,AL100,AM100,AN100,AO100,AP100,AQ100,AR100,AS100,AT100,AU100,AV100,AW100,AX100,AY100,AZ100,BA100,BB100,BC100,BD100,BE100,BF100,BG100,BH100,BI100,BJ100,BK100,BL100)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH97</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B100,AI100,AJ100,AK100,AL100,AM100,AN100,AO100,AP100,AQ100,AR100,AS100,AT100,AU100,AV100,AW100,AX100,AY100,AZ100,BA100,BB100,BC100,BD100,BE100,BF100,BG100,BH100,BI100,BJ100,BK100,BL100)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH97</v>
       </c>
       <c r="AI100" s="0" t="str">
         <f aca="false">IF(D100="y", " --"&amp;D$1,IF(NOT(ISBLANK(D100))," --"&amp;D$1&amp;" "&amp;D100,""))</f>
@@ -27558,13 +27637,13 @@
         <v/>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="n">
         <v>98</v>
       </c>
       <c r="AH101" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B101,AI101,AJ101,AK101,AL101,AM101,AN101,AO101,AP101,AQ101,AR101,AS101,AT101,AU101,AV101,AW101,AX101,AY101,AZ101,BA101,BB101,BC101,BD101,BE101,BF101,BG101,BH101,BI101,BJ101,BK101,BL101)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH98</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B101,AI101,AJ101,AK101,AL101,AM101,AN101,AO101,AP101,AQ101,AR101,AS101,AT101,AU101,AV101,AW101,AX101,AY101,AZ101,BA101,BB101,BC101,BD101,BE101,BF101,BG101,BH101,BI101,BJ101,BK101,BL101)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH98</v>
       </c>
       <c r="AI101" s="0" t="str">
         <f aca="false">IF(D101="y", " --"&amp;D$1,IF(NOT(ISBLANK(D101))," --"&amp;D$1&amp;" "&amp;D101,""))</f>
@@ -27683,13 +27762,13 @@
         <v/>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="n">
         <v>99</v>
       </c>
       <c r="AH102" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B102,AI102,AJ102,AK102,AL102,AM102,AN102,AO102,AP102,AQ102,AR102,AS102,AT102,AU102,AV102,AW102,AX102,AY102,AZ102,BA102,BB102,BC102,BD102,BE102,BF102,BG102,BH102,BI102,BJ102,BK102,BL102)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH99</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B102,AI102,AJ102,AK102,AL102,AM102,AN102,AO102,AP102,AQ102,AR102,AS102,AT102,AU102,AV102,AW102,AX102,AY102,AZ102,BA102,BB102,BC102,BD102,BE102,BF102,BG102,BH102,BI102,BJ102,BK102,BL102)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH99</v>
       </c>
       <c r="AI102" s="0" t="str">
         <f aca="false">IF(D102="y", " --"&amp;D$1,IF(NOT(ISBLANK(D102))," --"&amp;D$1&amp;" "&amp;D102,""))</f>
@@ -27808,13 +27887,13 @@
         <v/>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="n">
         <v>100</v>
       </c>
       <c r="AH103" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B103,AI103,AJ103,AK103,AL103,AM103,AN103,AO103,AP103,AQ103,AR103,AS103,AT103,AU103,AV103,AW103,AX103,AY103,AZ103,BA103,BB103,BC103,BD103,BE103,BF103,BG103,BH103,BI103,BJ103,BK103,BL103)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH100</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,B103,AI103,AJ103,AK103,AL103,AM103,AN103,AO103,AP103,AQ103,AR103,AS103,AT103,AU103,AV103,AW103,AX103,AY103,AZ103,BA103,BB103,BC103,BD103,BE103,BF103,BG103,BH103,BI103,BJ103,BK103,BL103)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH100</v>
       </c>
       <c r="AI103" s="0" t="str">
         <f aca="false">IF(D103="y", " --"&amp;D$1,IF(NOT(ISBLANK(D103))," --"&amp;D$1&amp;" "&amp;D103,""))</f>
@@ -27961,14 +28040,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="11" min="1" style="0" width="9.80566801619433"/>
+    <col collapsed="false" hidden="false" max="11" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="true" max="13" min="12" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="29" min="14" style="0" width="9.80566801619433"/>
+    <col collapsed="false" hidden="false" max="29" min="14" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="true" max="31" min="30" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="34" min="32" style="0" width="9.80566801619433"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="34" min="32" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="11.6275303643725"/>
     <col collapsed="false" hidden="true" max="67" min="36" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="68" style="0" width="9.80566801619433"/>
+    <col collapsed="false" hidden="false" max="1025" min="68" style="0" width="10.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27988,7 +28067,7 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
@@ -28000,10 +28079,10 @@
         <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>19</v>
@@ -28018,49 +28097,49 @@
         <v>27</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>20</v>
@@ -28069,12 +28148,12 @@
         <v>21</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="229.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
@@ -28083,13 +28162,13 @@
         <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>41</v>
@@ -28101,10 +28180,10 @@
         <v>62</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>50</v>
@@ -28119,64 +28198,64 @@
         <v>58</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28184,10 +28263,10 @@
         <v>1</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI3" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ3" s="0" t="str">
         <f aca="false">IF(C3="y", " --"&amp;C$1,IF(NOT(ISBLANK(C3))," --"&amp;C$1&amp;" "&amp;C3,""))</f>
@@ -28333,10 +28412,10 @@
         <v>68</v>
       </c>
       <c r="AC4" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI4" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ4" s="0" t="str">
         <f aca="false">IF(C4="y", " --"&amp;C$1,IF(NOT(ISBLANK(C4))," --"&amp;C$1&amp;" "&amp;C4,""))</f>
@@ -28482,10 +28561,10 @@
         <v>68</v>
       </c>
       <c r="AC5" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI5" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ5" s="0" t="str">
         <f aca="false">IF(C5="y", " --"&amp;C$1,IF(NOT(ISBLANK(C5))," --"&amp;C$1&amp;" "&amp;C5,""))</f>
@@ -28631,10 +28710,10 @@
         <v>68</v>
       </c>
       <c r="AC6" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI6" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ6" s="0" t="str">
         <f aca="false">IF(C6="y", " --"&amp;C$1,IF(NOT(ISBLANK(C6))," --"&amp;C$1&amp;" "&amp;C6,""))</f>
@@ -28780,10 +28859,10 @@
         <v>68</v>
       </c>
       <c r="AC7" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI7" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ7" s="0" t="str">
         <f aca="false">IF(C7="y", " --"&amp;C$1,IF(NOT(ISBLANK(C7))," --"&amp;C$1&amp;" "&amp;C7,""))</f>
@@ -28932,10 +29011,10 @@
         <v>68</v>
       </c>
       <c r="AC8" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI8" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ8" s="0" t="str">
         <f aca="false">IF(C8="y", " --"&amp;C$1,IF(NOT(ISBLANK(C8))," --"&amp;C$1&amp;" "&amp;C8,""))</f>
@@ -29084,10 +29163,10 @@
         <v>68</v>
       </c>
       <c r="AC9" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI9" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ9" s="0" t="str">
         <f aca="false">IF(C9="y", " --"&amp;C$1,IF(NOT(ISBLANK(C9))," --"&amp;C$1&amp;" "&amp;C9,""))</f>
@@ -29236,10 +29315,10 @@
         <v>68</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI10" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ10" s="0" t="str">
         <f aca="false">IF(C10="y", " --"&amp;C$1,IF(NOT(ISBLANK(C10))," --"&amp;C$1&amp;" "&amp;C10,""))</f>
@@ -29385,10 +29464,10 @@
         <v>68</v>
       </c>
       <c r="AC11" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI11" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ11" s="0" t="str">
         <f aca="false">IF(C11="y", " --"&amp;C$1,IF(NOT(ISBLANK(C11))," --"&amp;C$1&amp;" "&amp;C11,""))</f>
@@ -29537,10 +29616,10 @@
         <v>68</v>
       </c>
       <c r="AC12" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI12" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ12" s="0" t="str">
         <f aca="false">IF(C12="y", " --"&amp;C$1,IF(NOT(ISBLANK(C12))," --"&amp;C$1&amp;" "&amp;C12,""))</f>
@@ -29686,10 +29765,10 @@
         <v>68</v>
       </c>
       <c r="AC13" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI13" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ13" s="0" t="str">
         <f aca="false">IF(C13="y", " --"&amp;C$1,IF(NOT(ISBLANK(C13))," --"&amp;C$1&amp;" "&amp;C13,""))</f>
@@ -29835,10 +29914,10 @@
         <v>68</v>
       </c>
       <c r="AC14" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI14" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ14" s="0" t="str">
         <f aca="false">IF(C14="y", " --"&amp;C$1,IF(NOT(ISBLANK(C14))," --"&amp;C$1&amp;" "&amp;C14,""))</f>
@@ -29984,10 +30063,10 @@
         <v>68</v>
       </c>
       <c r="AC15" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI15" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ15" s="0" t="str">
         <f aca="false">IF(C15="y", " --"&amp;C$1,IF(NOT(ISBLANK(C15))," --"&amp;C$1&amp;" "&amp;C15,""))</f>
@@ -30133,10 +30212,10 @@
         <v>68</v>
       </c>
       <c r="AC16" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI16" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ16" s="0" t="str">
         <f aca="false">IF(C16="y", " --"&amp;C$1,IF(NOT(ISBLANK(C16))," --"&amp;C$1&amp;" "&amp;C16,""))</f>
@@ -30282,10 +30361,10 @@
         <v>68</v>
       </c>
       <c r="AC17" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI17" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ17" s="0" t="str">
         <f aca="false">IF(C17="y", " --"&amp;C$1,IF(NOT(ISBLANK(C17))," --"&amp;C$1&amp;" "&amp;C17,""))</f>
@@ -30431,10 +30510,10 @@
         <v>68</v>
       </c>
       <c r="AC18" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI18" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ18" s="0" t="str">
         <f aca="false">IF(C18="y", " --"&amp;C$1,IF(NOT(ISBLANK(C18))," --"&amp;C$1&amp;" "&amp;C18,""))</f>
@@ -30583,10 +30662,10 @@
         <v>68</v>
       </c>
       <c r="AC19" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI19" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ19" s="0" t="str">
         <f aca="false">IF(C19="y", " --"&amp;C$1,IF(NOT(ISBLANK(C19))," --"&amp;C$1&amp;" "&amp;C19,""))</f>
@@ -30735,10 +30814,10 @@
         <v>68</v>
       </c>
       <c r="AC20" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI20" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ20" s="0" t="str">
         <f aca="false">IF(C20="y", " --"&amp;C$1,IF(NOT(ISBLANK(C20))," --"&amp;C$1&amp;" "&amp;C20,""))</f>
@@ -30887,10 +30966,10 @@
         <v>68</v>
       </c>
       <c r="AC21" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI21" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ21" s="0" t="str">
         <f aca="false">IF(C21="y", " --"&amp;C$1,IF(NOT(ISBLANK(C21))," --"&amp;C$1&amp;" "&amp;C21,""))</f>
@@ -31039,10 +31118,10 @@
         <v>68</v>
       </c>
       <c r="AC22" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI22" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ22" s="0" t="str">
         <f aca="false">IF(C22="y", " --"&amp;C$1,IF(NOT(ISBLANK(C22))," --"&amp;C$1&amp;" "&amp;C22,""))</f>
@@ -31191,10 +31270,10 @@
         <v>68</v>
       </c>
       <c r="AC23" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI23" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ23" s="0" t="str">
         <f aca="false">IF(C23="y", " --"&amp;C$1,IF(NOT(ISBLANK(C23))," --"&amp;C$1&amp;" "&amp;C23,""))</f>
@@ -31343,10 +31422,10 @@
         <v>68</v>
       </c>
       <c r="AC24" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI24" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ24" s="0" t="str">
         <f aca="false">IF(C24="y", " --"&amp;C$1,IF(NOT(ISBLANK(C24))," --"&amp;C$1&amp;" "&amp;C24,""))</f>
@@ -31495,10 +31574,10 @@
         <v>68</v>
       </c>
       <c r="AC25" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI25" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ25" s="0" t="str">
         <f aca="false">IF(C25="y", " --"&amp;C$1,IF(NOT(ISBLANK(C25))," --"&amp;C$1&amp;" "&amp;C25,""))</f>
@@ -31647,10 +31726,10 @@
         <v>68</v>
       </c>
       <c r="AC26" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI26" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ26" s="0" t="str">
         <f aca="false">IF(C26="y", " --"&amp;C$1,IF(NOT(ISBLANK(C26))," --"&amp;C$1&amp;" "&amp;C26,""))</f>
@@ -31799,10 +31878,10 @@
         <v>68</v>
       </c>
       <c r="AC27" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI27" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ27" s="0" t="str">
         <f aca="false">IF(C27="y", " --"&amp;C$1,IF(NOT(ISBLANK(C27))," --"&amp;C$1&amp;" "&amp;C27,""))</f>
@@ -31951,10 +32030,10 @@
         <v>68</v>
       </c>
       <c r="AC28" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI28" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ28" s="0" t="str">
         <f aca="false">IF(C28="y", " --"&amp;C$1,IF(NOT(ISBLANK(C28))," --"&amp;C$1&amp;" "&amp;C28,""))</f>
@@ -32103,10 +32182,10 @@
         <v>68</v>
       </c>
       <c r="AC29" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI29" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ29" s="0" t="str">
         <f aca="false">IF(C29="y", " --"&amp;C$1,IF(NOT(ISBLANK(C29))," --"&amp;C$1&amp;" "&amp;C29,""))</f>
@@ -32255,10 +32334,10 @@
         <v>68</v>
       </c>
       <c r="AC30" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI30" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ30" s="0" t="str">
         <f aca="false">IF(C30="y", " --"&amp;C$1,IF(NOT(ISBLANK(C30))," --"&amp;C$1&amp;" "&amp;C30,""))</f>
@@ -32407,10 +32486,10 @@
         <v>68</v>
       </c>
       <c r="AC31" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI31" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ31" s="0" t="str">
         <f aca="false">IF(C31="y", " --"&amp;C$1,IF(NOT(ISBLANK(C31))," --"&amp;C$1&amp;" "&amp;C31,""))</f>
@@ -32559,10 +32638,10 @@
         <v>68</v>
       </c>
       <c r="AC32" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI32" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ32" s="0" t="str">
         <f aca="false">IF(C32="y", " --"&amp;C$1,IF(NOT(ISBLANK(C32))," --"&amp;C$1&amp;" "&amp;C32,""))</f>
@@ -32711,10 +32790,10 @@
         <v>68</v>
       </c>
       <c r="AC33" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI33" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ33" s="0" t="str">
         <f aca="false">IF(C33="y", " --"&amp;C$1,IF(NOT(ISBLANK(C33))," --"&amp;C$1&amp;" "&amp;C33,""))</f>
@@ -32863,10 +32942,10 @@
         <v>68</v>
       </c>
       <c r="AC34" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI34" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ34" s="0" t="str">
         <f aca="false">IF(C34="y", " --"&amp;C$1,IF(NOT(ISBLANK(C34))," --"&amp;C$1&amp;" "&amp;C34,""))</f>
@@ -33015,10 +33094,10 @@
         <v>68</v>
       </c>
       <c r="AC35" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI35" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ35" s="0" t="str">
         <f aca="false">IF(C35="y", " --"&amp;C$1,IF(NOT(ISBLANK(C35))," --"&amp;C$1&amp;" "&amp;C35,""))</f>
@@ -33167,10 +33246,10 @@
         <v>68</v>
       </c>
       <c r="AC36" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI36" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ36" s="0" t="str">
         <f aca="false">IF(C36="y", " --"&amp;C$1,IF(NOT(ISBLANK(C36))," --"&amp;C$1&amp;" "&amp;C36,""))</f>
@@ -33319,13 +33398,13 @@
         <v>68</v>
       </c>
       <c r="AC37" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AH37" s="0" t="s">
         <v>68</v>
       </c>
       <c r="AI37" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ37" s="0" t="str">
         <f aca="false">IF(C37="y", " --"&amp;C$1,IF(NOT(ISBLANK(C37))," --"&amp;C$1&amp;" "&amp;C37,""))</f>
@@ -33474,13 +33553,13 @@
         <v>68</v>
       </c>
       <c r="AC38" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AH38" s="0" t="s">
         <v>68</v>
       </c>
       <c r="AI38" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ38" s="0" t="str">
         <f aca="false">IF(C38="y", " --"&amp;C$1,IF(NOT(ISBLANK(C38))," --"&amp;C$1&amp;" "&amp;C38,""))</f>
@@ -33629,10 +33708,10 @@
         <v>68</v>
       </c>
       <c r="AC39" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI39" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ39" s="0" t="str">
         <f aca="false">IF(C39="y", " --"&amp;C$1,IF(NOT(ISBLANK(C39))," --"&amp;C$1&amp;" "&amp;C39,""))</f>
@@ -33781,10 +33860,10 @@
         <v>68</v>
       </c>
       <c r="AC40" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI40" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ40" s="0" t="str">
         <f aca="false">IF(C40="y", " --"&amp;C$1,IF(NOT(ISBLANK(C40))," --"&amp;C$1&amp;" "&amp;C40,""))</f>
@@ -33933,10 +34012,10 @@
         <v>68</v>
       </c>
       <c r="AC41" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI41" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ41" s="0" t="str">
         <f aca="false">IF(C41="y", " --"&amp;C$1,IF(NOT(ISBLANK(C41))," --"&amp;C$1&amp;" "&amp;C41,""))</f>
@@ -34085,10 +34164,10 @@
         <v>68</v>
       </c>
       <c r="AC42" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI42" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ42" s="0" t="str">
         <f aca="false">IF(C42="y", " --"&amp;C$1,IF(NOT(ISBLANK(C42))," --"&amp;C$1&amp;" "&amp;C42,""))</f>
@@ -34237,10 +34316,10 @@
         <v>68</v>
       </c>
       <c r="AC43" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI43" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ43" s="0" t="str">
         <f aca="false">IF(C43="y", " --"&amp;C$1,IF(NOT(ISBLANK(C43))," --"&amp;C$1&amp;" "&amp;C43,""))</f>
@@ -34389,10 +34468,10 @@
         <v>68</v>
       </c>
       <c r="AC44" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI44" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ44" s="0" t="str">
         <f aca="false">IF(C44="y", " --"&amp;C$1,IF(NOT(ISBLANK(C44))," --"&amp;C$1&amp;" "&amp;C44,""))</f>
@@ -34541,10 +34620,10 @@
         <v>68</v>
       </c>
       <c r="AC45" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AI45" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ45" s="0" t="str">
         <f aca="false">IF(C45="y", " --"&amp;C$1,IF(NOT(ISBLANK(C45))," --"&amp;C$1&amp;" "&amp;C45,""))</f>
@@ -34693,13 +34772,13 @@
         <v>68</v>
       </c>
       <c r="AC46" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AG46" s="0" t="n">
         <v>100</v>
       </c>
       <c r="AI46" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ46" s="0" t="str">
         <f aca="false">IF(C46="y", " --"&amp;C$1,IF(NOT(ISBLANK(C46))," --"&amp;C$1&amp;" "&amp;C46,""))</f>
@@ -34845,13 +34924,13 @@
         <v>68</v>
       </c>
       <c r="AC47" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AG47" s="0" t="n">
         <v>500</v>
       </c>
       <c r="AI47" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ47" s="0" t="str">
         <f aca="false">IF(C47="y", " --"&amp;C$1,IF(NOT(ISBLANK(C47))," --"&amp;C$1&amp;" "&amp;C47,""))</f>
@@ -34997,13 +35076,13 @@
         <v>68</v>
       </c>
       <c r="AC48" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AG48" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="AI48" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ48" s="0" t="str">
         <f aca="false">IF(C48="y", " --"&amp;C$1,IF(NOT(ISBLANK(C48))," --"&amp;C$1&amp;" "&amp;C48,""))</f>
@@ -35149,7 +35228,7 @@
         <v>68</v>
       </c>
       <c r="AC49" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AF49" s="0" t="n">
         <v>5000</v>
@@ -35158,7 +35237,7 @@
         <v>100</v>
       </c>
       <c r="AI49" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ49" s="0" t="str">
         <f aca="false">IF(C49="y", " --"&amp;C$1,IF(NOT(ISBLANK(C49))," --"&amp;C$1&amp;" "&amp;C49,""))</f>
@@ -35304,7 +35383,7 @@
         <v>68</v>
       </c>
       <c r="AC50" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AF50" s="0" t="n">
         <v>5000</v>
@@ -35313,7 +35392,7 @@
         <v>500</v>
       </c>
       <c r="AI50" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ50" s="0" t="str">
         <f aca="false">IF(C50="y", " --"&amp;C$1,IF(NOT(ISBLANK(C50))," --"&amp;C$1&amp;" "&amp;C50,""))</f>
@@ -35459,7 +35538,7 @@
         <v>68</v>
       </c>
       <c r="AC51" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AF51" s="0" t="n">
         <v>5000</v>
@@ -35468,7 +35547,7 @@
         <v>1000</v>
       </c>
       <c r="AI51" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ51" s="0" t="str">
         <f aca="false">IF(C51="y", " --"&amp;C$1,IF(NOT(ISBLANK(C51))," --"&amp;C$1&amp;" "&amp;C51,""))</f>
@@ -35617,7 +35696,7 @@
         <v>68</v>
       </c>
       <c r="AC52" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AF52" s="0" t="n">
         <v>5000</v>
@@ -35626,7 +35705,7 @@
         <v>100</v>
       </c>
       <c r="AI52" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ52" s="0" t="str">
         <f aca="false">IF(C52="y", " --"&amp;C$1,IF(NOT(ISBLANK(C52))," --"&amp;C$1&amp;" "&amp;C52,""))</f>
@@ -35775,7 +35854,7 @@
         <v>68</v>
       </c>
       <c r="AC53" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AF53" s="0" t="n">
         <v>5000</v>
@@ -35784,7 +35863,7 @@
         <v>100</v>
       </c>
       <c r="AI53" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ53" s="0" t="str">
         <f aca="false">IF(C53="y", " --"&amp;C$1,IF(NOT(ISBLANK(C53))," --"&amp;C$1&amp;" "&amp;C53,""))</f>
@@ -35933,7 +36012,7 @@
         <v>68</v>
       </c>
       <c r="AC54" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AF54" s="0" t="n">
         <v>5000</v>
@@ -35942,7 +36021,7 @@
         <v>100</v>
       </c>
       <c r="AI54" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ54" s="0" t="str">
         <f aca="false">IF(C54="y", " --"&amp;C$1,IF(NOT(ISBLANK(C54))," --"&amp;C$1&amp;" "&amp;C54,""))</f>
@@ -36091,7 +36170,7 @@
         <v>68</v>
       </c>
       <c r="AC55" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AF55" s="0" t="n">
         <v>5000</v>
@@ -36100,7 +36179,7 @@
         <v>100</v>
       </c>
       <c r="AI55" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ55" s="0" t="str">
         <f aca="false">IF(C55="y", " --"&amp;C$1,IF(NOT(ISBLANK(C55))," --"&amp;C$1&amp;" "&amp;C55,""))</f>
@@ -36249,7 +36328,7 @@
         <v>68</v>
       </c>
       <c r="AC56" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AF56" s="0" t="n">
         <v>5000</v>
@@ -36258,7 +36337,7 @@
         <v>100</v>
       </c>
       <c r="AI56" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AJ56" s="0" t="str">
         <f aca="false">IF(C56="y", " --"&amp;C$1,IF(NOT(ISBLANK(C56))," --"&amp;C$1&amp;" "&amp;C56,""))</f>

</xml_diff>

<commit_message>
error, missing accommodation for 32..96 x 2 category data
</commit_message>
<xml_diff>
--- a/convParameters.xlsx
+++ b/convParameters.xlsx
@@ -14400,8 +14400,8 @@
   </sheetPr>
   <dimension ref="A1:BK103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB44" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD50" activeCellId="0" sqref="AD50"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC44" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AH53" activeCellId="0" sqref="AH53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20818,8 +20818,8 @@
         <v>68</v>
       </c>
       <c r="AH47" s="0" t="str">
-        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment.sh ",$A$2,B47,AI47,AJ47,AK47,AL47,AM47,AN47,AO47,AP47,AQ47,AR47,AS47,AT47,AU47,AV47,AW47,AX47,AY47,AZ47,BA47,BB47,BC47,BD47,BE47,BF47,BG47,BH47,BI47,BJ47,BK47,BL47)</f>
-        <v>docker exec -it $IMAGE ./convExperiment.sh EH44--learningRate 0.001--minLR 0.0000001--standardize--zca--lecunlcn --hiddenSize  '{400}'--batchNorm--dropout</v>
+        <f aca="false">CONCATENATE("docker exec -it $IMAGE ./convExperiment2.sh ",$A$2,"_2_",B47,AI47,AJ47,AK47,AL47,AM47,AN47,AO47,AP47,AQ47,AR47,AS47,AT47,AU47,AV47,AW47,AX47,AY47,AZ47,BA47,BB47,BC47,BD47,BE47,BF47,BG47,BH47,BI47,BJ47,BK47,BL47)</f>
+        <v>docker exec -it $IMAGE ./convExperiment2.sh EH_2_44--learningRate 0.001--minLR 0.0000001--standardize--zca--lecunlcn --hiddenSize  '{400}'--batchNorm--dropout</v>
       </c>
       <c r="AI47" s="0" t="str">
         <f aca="false">IF(D47="y", " --"&amp;D$1,IF(NOT(ISBLANK(D47))," --"&amp;D$1&amp;" "&amp;D47,""))</f>

</xml_diff>